<commit_message>
add D3 and Hudgson 2023 trait database
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
     <t>database</t>
   </si>
@@ -328,43 +328,46 @@
     <t>Disturbance.Severity</t>
   </si>
   <si>
-    <t xml:space="preserve">Disturbance severity value for the whole community</t>
+    <t xml:space="preserve">Disturbance severity (proportional, 0-1); mean value for the whole community</t>
   </si>
   <si>
     <t>Disturbance.Severity.herblayer</t>
   </si>
   <si>
-    <t xml:space="preserve">Disturbance severity value at the herb layer</t>
+    <t xml:space="preserve">Disturbance severity (proportional, 0-1); mean value at the herb layer</t>
   </si>
   <si>
     <t>Disturbance.Frequency</t>
   </si>
   <si>
-    <t xml:space="preserve">Disturbance frequency value for the whole community</t>
+    <t xml:space="preserve">Mean value of disturbance return time (years) for the whole community</t>
+  </si>
+  <si>
+    <t>years</t>
   </si>
   <si>
     <t>Disturbance.Frequency.herblayer</t>
   </si>
   <si>
-    <t xml:space="preserve">Disturbance frequency value at the herb layer</t>
+    <t xml:space="preserve">Mean value of disturbance return time (years) at the herb layer</t>
   </si>
   <si>
     <t>Mowing.Frequency</t>
   </si>
   <si>
-    <t xml:space="preserve">Mowing frequency value</t>
+    <t xml:space="preserve">Mean value for the mowing return time (years) at the herb layer</t>
   </si>
   <si>
     <t>Grazing.Pressure</t>
   </si>
   <si>
-    <t xml:space="preserve">Grazing pressure value</t>
+    <t xml:space="preserve">Grazing pressure mean value (proportional, 0-1)</t>
   </si>
   <si>
     <t>Soil.Disturbance</t>
   </si>
   <si>
-    <t xml:space="preserve">Soil disturbance value</t>
+    <t xml:space="preserve">Soil disturbance mean value (proportional, 0-1)</t>
   </si>
   <si>
     <t>SPVignes</t>
@@ -541,6 +544,282 @@
     <t>PV.butterflies</t>
   </si>
   <si>
+    <t>dcube</t>
+  </si>
+  <si>
+    <t>fruit_type</t>
+  </si>
+  <si>
+    <t>fruit.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the ecological characteristics of the fruit that are related to seed dispersal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 classes</t>
+  </si>
+  <si>
+    <t>dia_type</t>
+  </si>
+  <si>
+    <t>dia.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the morphological structure that acts as the diaspore, i.e. the diasporsal unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 classes</t>
+  </si>
+  <si>
+    <t>dia_exposure</t>
+  </si>
+  <si>
+    <t>dia.exposure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diaspore exposure, accessibility of dispersal vectors to the diaspores within the infructescence;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 classes</t>
+  </si>
+  <si>
+    <t>dia_hetero</t>
+  </si>
+  <si>
+    <t>dia.hetero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heterodiaspory, a heterodiaspore species features more than one diaspore type</t>
+  </si>
+  <si>
+    <t>(0,1)</t>
+  </si>
+  <si>
+    <t>dia_app_nutrient</t>
+  </si>
+  <si>
+    <t>dia.app.nutrient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrients, indicator for dysochory and endozoochory</t>
+  </si>
+  <si>
+    <t>dia_app_elon</t>
+  </si>
+  <si>
+    <t>dia.app.elon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elongated appendages, indicator for anemochory and epizoocccchory</t>
+  </si>
+  <si>
+    <t>dia_app_hook</t>
+  </si>
+  <si>
+    <t>dia.app.hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hooked appendages, indicator for epizoochory</t>
+  </si>
+  <si>
+    <t>dia_app_muci</t>
+  </si>
+  <si>
+    <t>dia.app.muci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mucilaginous surface, indicator for epizoochory and endozoochory</t>
+  </si>
+  <si>
+    <t>dia_mass</t>
+  </si>
+  <si>
+    <t>dia.mass.mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore mass, weight of one diaspore including all appendages</t>
+  </si>
+  <si>
+    <t>dia_surfacestructure</t>
+  </si>
+  <si>
+    <t>dia.surfacestructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore surface structure, smoothness of a diaspore's surface based on images of the diaspores. very smooth surface =1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score (0-1)</t>
+  </si>
+  <si>
+    <t>dia_length</t>
+  </si>
+  <si>
+    <t>dia.length.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore length, i.e. the longest axis including all appendages</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>dia_width</t>
+  </si>
+  <si>
+    <t>dia.width.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore width, i.e. the second longest axis perpendicular to length, including all appendages</t>
+  </si>
+  <si>
+    <t>dia_height</t>
+  </si>
+  <si>
+    <t>dia.height.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore height, i.e. the shortest axis perpendicular to length and width, including all appendages</t>
+  </si>
+  <si>
+    <t>dia_shape</t>
+  </si>
+  <si>
+    <t>dia.shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore shape, deviation of a diaspore's shape from a sphere in three dimension; sphere =0</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>dia_form</t>
+  </si>
+  <si>
+    <t>dia.form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore form, form of diaspore in categories</t>
+  </si>
+  <si>
+    <t>vterm</t>
+  </si>
+  <si>
+    <t>term.velocity.m.s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminal velocity, maximum speed of a failing diaspore in still air</t>
+  </si>
+  <si>
+    <t>m.s-1</t>
+  </si>
+  <si>
+    <t>rank_ane</t>
+  </si>
+  <si>
+    <t>rank.ane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anemochory ranking index, assess how well a species is adapted to anemochory (wind dispersal)</t>
+  </si>
+  <si>
+    <t>rank_hydro</t>
+  </si>
+  <si>
+    <t>rank.hydro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrochory ranking index, assess how well a species is adapted to hydrochory (water dispersal)</t>
+  </si>
+  <si>
+    <t>rank_epi_wool</t>
+  </si>
+  <si>
+    <t>rank.epi.wool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epizoochory ranking index, assess how well a species is adapted to epizoochory (external animal dispersal)</t>
+  </si>
+  <si>
+    <t>diaspore_seeds_class</t>
+  </si>
+  <si>
+    <t>diaspore.seeds.class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore seed class</t>
+  </si>
+  <si>
+    <t>Hodgson_2023</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>SLA.mm2.mg-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific leaf area</t>
+  </si>
+  <si>
+    <t>mm2.mg-1</t>
+  </si>
+  <si>
+    <t>ARNODE</t>
+  </si>
+  <si>
+    <t>Arnode.mm2.mm-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area per node/thickness</t>
+  </si>
+  <si>
+    <t>mm2.mm-1</t>
+  </si>
+  <si>
+    <t>LOGCANH</t>
+  </si>
+  <si>
+    <t>Log2.canopy.height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy height (converted to log2 bins)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log 2 bins cm</t>
+  </si>
+  <si>
+    <t>LOGCAND</t>
+  </si>
+  <si>
+    <t>Log2.canopy.diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy diameter (converted to log2 bins)</t>
+  </si>
+  <si>
+    <t>VEGPROP</t>
+  </si>
+  <si>
+    <t>Vegprop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetative propagation  of perennials</t>
+  </si>
+  <si>
+    <t>LIFEHIST</t>
+  </si>
+  <si>
+    <t>Lifehist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annual, herbaceous perennial, wood perennial, biennial</t>
+  </si>
+  <si>
     <t>Database</t>
   </si>
   <si>
@@ -559,7 +838,7 @@
     <t>https://www.tela-botanica.org/projets/phytosociologie/porte-documents/</t>
   </si>
   <si>
-    <t>baseflor.xlsx</t>
+    <t>CATMINAT/baseflor.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Enquist BJ, Condit R, Peet RK, Schildhauer M, Thiers BM. (2016) Cyberinfrastructure for an integrated botanical information network to investigate the ecological impacts of global climate change on plant biodiversity. PeerJ Preprints 4:e2615v2</t>
@@ -611,6 +890,12 @@
   </si>
   <si>
     <t xml:space="preserve">Valeurs polliniques estimees.csv</t>
+  </si>
+  <si>
+    <t>Hintze</t>
+  </si>
+  <si>
+    <t>1-s2.0-S1433831913000218-mmc1.txt</t>
   </si>
   <si>
     <t>LEDA</t>
@@ -771,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -783,13 +1068,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
@@ -799,15 +1078,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1334,7 +1609,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1383,7 +1658,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1392,14 +1667,14 @@
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1408,8 +1683,8 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1484,8 +1759,6 @@
       <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9"/>
-      <c r="E9"/>
       <c r="F9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1500,8 +1773,6 @@
       <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10"/>
-      <c r="E10"/>
       <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1516,8 +1787,6 @@
       <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
       <c r="F11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1532,8 +1801,6 @@
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12" t="s">
         <v>31</v>
       </c>
@@ -1548,8 +1815,6 @@
       <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
       <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1564,8 +1829,6 @@
       <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D14"/>
-      <c r="E14"/>
       <c r="F14" t="s">
         <v>16</v>
       </c>
@@ -1580,8 +1843,6 @@
       <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="D15"/>
-      <c r="E15"/>
       <c r="F15" s="6" t="s">
         <v>9</v>
       </c>
@@ -1635,10 +1896,10 @@
       <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1652,7 +1913,7 @@
       <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1739,7 +2000,7 @@
       <c r="E26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1770,7 +2031,7 @@
       <c r="C28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2132,16 +2393,15 @@
       <c r="A50" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E50"/>
       <c r="F50" s="6" t="s">
         <v>59</v>
       </c>
@@ -2150,13 +2410,13 @@
       <c r="A51" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="9" t="s">
         <v>105</v>
       </c>
       <c r="F51" s="6" t="s">
@@ -2167,14 +2427,17 @@
       <c r="A52" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="9" t="s">
         <v>107</v>
+      </c>
+      <c r="E52" t="s">
+        <v>108</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>59</v>
@@ -2184,14 +2447,17 @@
       <c r="A53" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E53" t="s">
         <v>108</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>59</v>
@@ -2201,16 +2467,18 @@
       <c r="A54" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E54"/>
+      <c r="C54" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
       <c r="F54" s="6" t="s">
         <v>59</v>
       </c>
@@ -2219,16 +2487,15 @@
       <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E55"/>
+      <c r="C55" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="F55" s="6" t="s">
         <v>59</v>
       </c>
@@ -2237,33 +2504,32 @@
       <c r="A56" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="11" t="s">
+      <c r="B56" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E56"/>
+      <c r="C56" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="F56" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>59</v>
@@ -2271,29 +2537,27 @@
     </row>
     <row r="58" ht="14.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58"/>
-      <c r="E58"/>
+        <v>121</v>
+      </c>
       <c r="F58" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" s="14" t="s">
         <v>122</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>9</v>
@@ -2301,13 +2565,13 @@
     </row>
     <row r="60" ht="14.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="14" t="s">
         <v>124</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>9</v>
@@ -2315,13 +2579,13 @@
     </row>
     <row r="61" ht="14.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
-      </c>
-      <c r="C61" s="14" t="s">
         <v>126</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>9</v>
@@ -2329,13 +2593,13 @@
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
-      </c>
-      <c r="C62" s="14" t="s">
         <v>128</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>9</v>
@@ -2343,12 +2607,12 @@
     </row>
     <row r="63" ht="14.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F63" s="6" t="s">
@@ -2357,119 +2621,119 @@
     </row>
     <row r="64" ht="15">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" ht="15">
+      <c r="A65" t="s">
         <v>131</v>
       </c>
-      <c r="C64" t="s">
-        <v>132</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25">
-      <c r="A65" t="s">
-        <v>130</v>
-      </c>
       <c r="B65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" t="s">
+        <v>138</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" ht="15">
+      <c r="A66" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" t="s">
+        <v>140</v>
+      </c>
+      <c r="D66" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" ht="15">
+      <c r="A67" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" t="s">
+        <v>143</v>
+      </c>
+      <c r="D67" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C65" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" t="s">
-        <v>137</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" ht="14.25">
-      <c r="A66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" t="s">
-        <v>138</v>
-      </c>
-      <c r="C66" t="s">
-        <v>139</v>
-      </c>
-      <c r="D66" t="s">
-        <v>140</v>
-      </c>
-      <c r="E66" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25">
-      <c r="A67" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" t="s">
-        <v>141</v>
-      </c>
-      <c r="C67" t="s">
-        <v>142</v>
-      </c>
-      <c r="D67" t="s">
-        <v>143</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="F67" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" ht="14.25">
+    <row r="68" ht="15">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>134</v>
+        <v>147</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" ht="14.25">
+    <row r="69" ht="15">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E69" s="16" t="s">
         <v>150</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>59</v>
@@ -2477,29 +2741,28 @@
     </row>
     <row r="70" ht="14.25">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
-      </c>
-      <c r="C70" s="17" t="s">
         <v>153</v>
       </c>
+      <c r="C70" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="D70" s="2"/>
-      <c r="E70"/>
       <c r="F70" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>154</v>
-      </c>
-      <c r="C71" s="14" t="s">
         <v>155</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>9</v>
@@ -2507,28 +2770,27 @@
     </row>
     <row r="72" ht="14.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72"/>
+        <v>157</v>
+      </c>
       <c r="F72" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>157</v>
-      </c>
-      <c r="C73" s="14" t="s">
         <v>158</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="E73" t="s">
         <v>31</v>
@@ -2539,13 +2801,13 @@
     </row>
     <row r="74" ht="14.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
-      </c>
-      <c r="C74" s="14" t="s">
         <v>160</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="E74" t="s">
         <v>31</v>
@@ -2556,58 +2818,55 @@
     </row>
     <row r="75" ht="14.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E75"/>
+        <v>162</v>
+      </c>
       <c r="F75" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
-      </c>
-      <c r="C76" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="E76"/>
+      <c r="C76" s="6" t="s">
+        <v>164</v>
+      </c>
       <c r="F76" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>164</v>
-      </c>
-      <c r="C77" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E77"/>
+      <c r="C77" s="6" t="s">
+        <v>166</v>
+      </c>
       <c r="F77" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
-      </c>
-      <c r="C78" s="14" t="s">
         <v>167</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>31</v>
@@ -2618,13 +2877,13 @@
     </row>
     <row r="79" ht="14.25">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
-      </c>
-      <c r="C79" s="14" t="s">
         <v>169</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>31</v>
@@ -2635,13 +2894,13 @@
     </row>
     <row r="80" ht="14.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
-      </c>
-      <c r="C80" s="14" t="s">
         <v>171</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="E80" t="s">
         <v>31</v>
@@ -2652,13 +2911,13 @@
     </row>
     <row r="81" ht="14.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>172</v>
-      </c>
-      <c r="C81" s="14" t="s">
         <v>173</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>31</v>
@@ -2667,9 +2926,536 @@
         <v>59</v>
       </c>
     </row>
+    <row r="82" ht="14.25">
+      <c r="A82" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E82" t="s">
+        <v>179</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25">
+      <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D83" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" t="s">
+        <v>183</v>
+      </c>
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25">
+      <c r="A84" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D84" t="s">
+        <v>186</v>
+      </c>
+      <c r="E84" t="s">
+        <v>187</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" ht="14.25">
+      <c r="A85" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" t="s">
+        <v>188</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D85" t="s">
+        <v>190</v>
+      </c>
+      <c r="E85" t="s">
+        <v>191</v>
+      </c>
+      <c r="F85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" ht="14.25">
+      <c r="A86" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" t="s">
+        <v>192</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F86" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" ht="14.25">
+      <c r="A87" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" t="s">
+        <v>195</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" ht="14.25">
+      <c r="A88" t="s">
+        <v>175</v>
+      </c>
+      <c r="B88" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25">
+      <c r="A89" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D89" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25">
+      <c r="A90" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" t="s">
+        <v>204</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D90" t="s">
+        <v>206</v>
+      </c>
+      <c r="E90" t="s">
+        <v>73</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" ht="14.25">
+      <c r="A91" t="s">
+        <v>175</v>
+      </c>
+      <c r="B91" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E91" t="s">
+        <v>210</v>
+      </c>
+      <c r="F91" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" ht="14.25">
+      <c r="A92" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E92" t="s">
+        <v>214</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" ht="14.25">
+      <c r="A93" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93" t="s">
+        <v>215</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E93" t="s">
+        <v>214</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" ht="14.25">
+      <c r="A94" t="s">
+        <v>175</v>
+      </c>
+      <c r="B94" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D94" t="s">
+        <v>220</v>
+      </c>
+      <c r="E94" t="s">
+        <v>214</v>
+      </c>
+      <c r="F94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" ht="14.25">
+      <c r="A95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" t="s">
+        <v>221</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D95" t="s">
+        <v>223</v>
+      </c>
+      <c r="E95" t="s">
+        <v>224</v>
+      </c>
+      <c r="F95" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" ht="14.25">
+      <c r="A96" t="s">
+        <v>175</v>
+      </c>
+      <c r="B96" t="s">
+        <v>225</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D96" t="s">
+        <v>227</v>
+      </c>
+      <c r="E96" t="s">
+        <v>187</v>
+      </c>
+      <c r="F96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" ht="14.25">
+      <c r="A97" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D97" t="s">
+        <v>230</v>
+      </c>
+      <c r="E97" t="s">
+        <v>231</v>
+      </c>
+      <c r="F97" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" ht="14.25">
+      <c r="A98" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" t="s">
+        <v>232</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D98" t="s">
+        <v>234</v>
+      </c>
+      <c r="E98" t="s">
+        <v>210</v>
+      </c>
+      <c r="F98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25">
+      <c r="A99" t="s">
+        <v>175</v>
+      </c>
+      <c r="B99" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D99" t="s">
+        <v>237</v>
+      </c>
+      <c r="E99" t="s">
+        <v>210</v>
+      </c>
+      <c r="F99" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25">
+      <c r="A100" t="s">
+        <v>175</v>
+      </c>
+      <c r="B100" t="s">
+        <v>238</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D100" t="s">
+        <v>240</v>
+      </c>
+      <c r="E100" t="s">
+        <v>210</v>
+      </c>
+      <c r="F100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" ht="14.25">
+      <c r="A101" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" t="s">
+        <v>241</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D101" t="s">
+        <v>243</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" ht="14.25">
+      <c r="A102" t="s">
+        <v>244</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" ht="14.25">
+      <c r="A103" t="s">
+        <v>244</v>
+      </c>
+      <c r="B103" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" ht="14.25">
+      <c r="A104" t="s">
+        <v>244</v>
+      </c>
+      <c r="B104" t="s">
+        <v>253</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E104" t="s">
+        <v>256</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" ht="14.25">
+      <c r="A105" t="s">
+        <v>244</v>
+      </c>
+      <c r="B105" t="s">
+        <v>257</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E105" t="s">
+        <v>256</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" ht="14.25">
+      <c r="A106" t="s">
+        <v>244</v>
+      </c>
+      <c r="B106" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" t="s">
+        <v>261</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" ht="14.25">
+      <c r="A107" t="s">
+        <v>244</v>
+      </c>
+      <c r="B107" t="s">
+        <v>263</v>
+      </c>
+      <c r="C107" t="s">
+        <v>264</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" ht="14.25">
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" ht="14.25">
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" ht="14.25">
+      <c r="E110" s="6"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:F81" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="A2:A81"/>
+  <sortState ref="A2:F89" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A89"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2692,156 +3478,162 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="D12" s="21"/>
+      <c r="A12" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:D10" columnSort="0">

</xml_diff>

<commit_message>
feat: merge traits and draft exploration
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="295">
   <si>
     <t>database</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>Efficient.dispersal.mode</t>
-  </si>
-  <si>
-    <t>class</t>
   </si>
   <si>
     <t xml:space="preserve">Dispersal distance class (1-6)</t>
@@ -1056,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1081,10 +1078,6 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
@@ -1609,7 +1602,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2365,9 +2358,6 @@
       <c r="C48" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E48" t="s">
-        <v>97</v>
-      </c>
       <c r="F48" s="6" t="s">
         <v>9</v>
       </c>
@@ -2377,67 +2367,67 @@
         <v>88</v>
       </c>
       <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="E49" t="s">
         <v>99</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" ht="28.5">
+      <c r="A50" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25">
-      <c r="A50" t="s">
+      <c r="B50" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="C50" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D50" s="9" t="s">
+      <c r="F50" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" ht="28.5">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25">
-      <c r="A51" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="10" t="s">
+      <c r="C51" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D51" s="9" t="s">
+      <c r="F51" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" ht="28.5">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25">
-      <c r="A52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="10" t="s">
+      <c r="C52" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D52" s="9" t="s">
+      <c r="E52" t="s">
         <v>107</v>
-      </c>
-      <c r="E52" t="s">
-        <v>108</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>59</v>
@@ -2445,39 +2435,39 @@
     </row>
     <row r="53" ht="14.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" s="9" t="s">
+      <c r="E53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" ht="28.5">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E53" t="s">
-        <v>108</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25">
-      <c r="A54" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="10" t="s">
+      <c r="C54" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="E54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>59</v>
@@ -2485,16 +2475,16 @@
     </row>
     <row r="55" ht="14.25">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>59</v>
@@ -2502,16 +2492,16 @@
     </row>
     <row r="56" ht="14.25">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B56" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>59</v>
@@ -2519,17 +2509,17 @@
     </row>
     <row r="57" ht="14.25">
       <c r="A57" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" t="s">
         <v>118</v>
-      </c>
-      <c r="C57" t="s">
-        <v>119</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>59</v>
@@ -2537,13 +2527,13 @@
     </row>
     <row r="58" ht="14.25">
       <c r="A58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>9</v>
@@ -2551,13 +2541,13 @@
     </row>
     <row r="59" ht="14.25">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>9</v>
@@ -2565,13 +2555,13 @@
     </row>
     <row r="60" ht="14.25">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>9</v>
@@ -2579,13 +2569,13 @@
     </row>
     <row r="61" ht="14.25">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>9</v>
@@ -2593,13 +2583,13 @@
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>9</v>
@@ -2607,10 +2597,10 @@
     </row>
     <row r="63" ht="14.25">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>8</v>
@@ -2621,19 +2611,19 @@
     </row>
     <row r="64" ht="15">
       <c r="A64" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64" t="s">
         <v>131</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>132</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>59</v>
@@ -2641,16 +2631,16 @@
     </row>
     <row r="65" ht="15">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" t="s">
         <v>136</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>137</v>
-      </c>
-      <c r="D65" t="s">
-        <v>138</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>71</v>
@@ -2661,16 +2651,16 @@
     </row>
     <row r="66" ht="15">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" t="s">
         <v>139</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>140</v>
-      </c>
-      <c r="D66" t="s">
-        <v>141</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>71</v>
@@ -2681,19 +2671,19 @@
     </row>
     <row r="67" ht="15">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" t="s">
         <v>142</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>143</v>
       </c>
-      <c r="D67" t="s">
-        <v>144</v>
-      </c>
       <c r="E67" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>59</v>
@@ -2701,19 +2691,19 @@
     </row>
     <row r="68" ht="15">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B68" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" t="s">
         <v>145</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="E68" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>59</v>
@@ -2721,19 +2711,19 @@
     </row>
     <row r="69" ht="15">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
         <v>148</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>59</v>
@@ -2741,13 +2731,13 @@
     </row>
     <row r="70" ht="14.25">
       <c r="A70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" t="s">
         <v>152</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="D70" s="2"/>
       <c r="F70" s="6" t="s">
@@ -2756,13 +2746,13 @@
     </row>
     <row r="71" ht="14.25">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>9</v>
@@ -2770,13 +2760,13 @@
     </row>
     <row r="72" ht="14.25">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>9</v>
@@ -2784,13 +2774,13 @@
     </row>
     <row r="73" ht="14.25">
       <c r="A73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="E73" t="s">
         <v>31</v>
@@ -2801,13 +2791,13 @@
     </row>
     <row r="74" ht="14.25">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s">
+        <v>159</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="E74" t="s">
         <v>31</v>
@@ -2818,13 +2808,13 @@
     </row>
     <row r="75" ht="14.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>9</v>
@@ -2832,13 +2822,13 @@
     </row>
     <row r="76" ht="14.25">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>9</v>
@@ -2846,13 +2836,13 @@
     </row>
     <row r="77" ht="14.25">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B77" t="s">
+        <v>164</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>9</v>
@@ -2860,13 +2850,13 @@
     </row>
     <row r="78" ht="14.25">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>31</v>
@@ -2877,13 +2867,13 @@
     </row>
     <row r="79" ht="14.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>31</v>
@@ -2894,13 +2884,13 @@
     </row>
     <row r="80" ht="14.25">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="E80" t="s">
         <v>31</v>
@@ -2911,13 +2901,13 @@
     </row>
     <row r="81" ht="14.25">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B81" t="s">
+        <v>172</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>31</v>
@@ -2928,19 +2918,19 @@
     </row>
     <row r="82" ht="14.25">
       <c r="A82" t="s">
+        <v>174</v>
+      </c>
+      <c r="B82" t="s">
         <v>175</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E82" t="s">
         <v>178</v>
-      </c>
-      <c r="E82" t="s">
-        <v>179</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>9</v>
@@ -2948,19 +2938,19 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B83" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="D83" t="s">
         <v>181</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>182</v>
-      </c>
-      <c r="E83" t="s">
-        <v>183</v>
       </c>
       <c r="F83" t="s">
         <v>9</v>
@@ -2968,19 +2958,19 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="D84" t="s">
         <v>185</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>186</v>
-      </c>
-      <c r="E84" t="s">
-        <v>187</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>9</v>
@@ -2989,19 +2979,19 @@
     </row>
     <row r="85" ht="14.25">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="D85" t="s">
         <v>189</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>190</v>
-      </c>
-      <c r="E85" t="s">
-        <v>191</v>
       </c>
       <c r="F85" t="s">
         <v>81</v>
@@ -3009,19 +2999,19 @@
     </row>
     <row r="86" ht="14.25">
       <c r="A86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="D86" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="E86" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F86" t="s">
         <v>81</v>
@@ -3029,19 +3019,19 @@
     </row>
     <row r="87" ht="14.25">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="D87" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="E87" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>81</v>
@@ -3049,19 +3039,19 @@
     </row>
     <row r="88" ht="14.25">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="D88" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="E88" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>81</v>
@@ -3069,19 +3059,19 @@
     </row>
     <row r="89" ht="14.25">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B89" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="D89" t="s">
         <v>202</v>
       </c>
-      <c r="D89" t="s">
-        <v>203</v>
-      </c>
       <c r="E89" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>81</v>
@@ -3089,16 +3079,16 @@
     </row>
     <row r="90" ht="14.25">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B90" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="D90" t="s">
         <v>205</v>
-      </c>
-      <c r="D90" t="s">
-        <v>206</v>
       </c>
       <c r="E90" t="s">
         <v>73</v>
@@ -3109,19 +3099,19 @@
     </row>
     <row r="91" ht="14.25">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
+        <v>206</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="D91" t="s">
         <v>208</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>209</v>
-      </c>
-      <c r="E91" t="s">
-        <v>210</v>
       </c>
       <c r="F91" t="s">
         <v>59</v>
@@ -3129,19 +3119,19 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
+        <v>210</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="D92" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="E92" t="s">
         <v>213</v>
-      </c>
-      <c r="E92" t="s">
-        <v>214</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>59</v>
@@ -3149,19 +3139,19 @@
     </row>
     <row r="93" ht="14.25">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
+        <v>214</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="D93" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="E93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>59</v>
@@ -3169,19 +3159,19 @@
     </row>
     <row r="94" ht="14.25">
       <c r="A94" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B94" t="s">
+        <v>217</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="D94" t="s">
         <v>219</v>
       </c>
-      <c r="D94" t="s">
-        <v>220</v>
-      </c>
       <c r="E94" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F94" t="s">
         <v>59</v>
@@ -3189,19 +3179,19 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="D95" t="s">
         <v>222</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>223</v>
-      </c>
-      <c r="E95" t="s">
-        <v>224</v>
       </c>
       <c r="F95" t="s">
         <v>59</v>
@@ -3209,19 +3199,19 @@
     </row>
     <row r="96" ht="14.25">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="D96" t="s">
         <v>226</v>
       </c>
-      <c r="D96" t="s">
-        <v>227</v>
-      </c>
       <c r="E96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F96" t="s">
         <v>9</v>
@@ -3229,19 +3219,19 @@
     </row>
     <row r="97" ht="14.25">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B97" t="s">
+        <v>227</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="D97" t="s">
         <v>229</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>230</v>
-      </c>
-      <c r="E97" t="s">
-        <v>231</v>
       </c>
       <c r="F97" t="s">
         <v>59</v>
@@ -3249,19 +3239,19 @@
     </row>
     <row r="98" ht="14.25">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="D98" t="s">
         <v>233</v>
       </c>
-      <c r="D98" t="s">
-        <v>234</v>
-      </c>
       <c r="E98" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F98" t="s">
         <v>59</v>
@@ -3269,19 +3259,19 @@
     </row>
     <row r="99" ht="14.25">
       <c r="A99" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="D99" t="s">
         <v>236</v>
       </c>
-      <c r="D99" t="s">
-        <v>237</v>
-      </c>
       <c r="E99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F99" t="s">
         <v>59</v>
@@ -3289,19 +3279,19 @@
     </row>
     <row r="100" ht="14.25">
       <c r="A100" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B100" t="s">
+        <v>237</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="D100" t="s">
         <v>239</v>
       </c>
-      <c r="D100" t="s">
-        <v>240</v>
-      </c>
       <c r="E100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F100" t="s">
         <v>59</v>
@@ -3309,16 +3299,16 @@
     </row>
     <row r="101" ht="14.25">
       <c r="A101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B101" t="s">
+        <v>240</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="D101" t="s">
         <v>242</v>
-      </c>
-      <c r="D101" t="s">
-        <v>243</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>59</v>
@@ -3326,19 +3316,19 @@
     </row>
     <row r="102" ht="14.25">
       <c r="A102" t="s">
+        <v>243</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C102" s="12" t="s">
+      <c r="D102" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="E102" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>59</v>
@@ -3346,19 +3336,19 @@
     </row>
     <row r="103" ht="14.25">
       <c r="A103" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B103" t="s">
+        <v>248</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="D103" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="E103" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>59</v>
@@ -3366,19 +3356,19 @@
     </row>
     <row r="104" ht="14.25">
       <c r="A104" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B104" t="s">
+        <v>252</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="D104" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D104" s="6" t="s">
+      <c r="E104" t="s">
         <v>255</v>
-      </c>
-      <c r="E104" t="s">
-        <v>256</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>59</v>
@@ -3386,19 +3376,19 @@
     </row>
     <row r="105" ht="14.25">
       <c r="A105" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B105" t="s">
+        <v>256</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="D105" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D105" s="6" t="s">
-        <v>259</v>
-      </c>
       <c r="E105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>59</v>
@@ -3406,19 +3396,19 @@
     </row>
     <row r="106" ht="14.25">
       <c r="A106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B106" t="s">
+        <v>259</v>
+      </c>
+      <c r="C106" t="s">
         <v>260</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="D106" s="6" t="s">
-        <v>262</v>
-      </c>
       <c r="E106" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>81</v>
@@ -3426,19 +3416,19 @@
     </row>
     <row r="107" ht="14.25">
       <c r="A107" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B107" t="s">
+        <v>262</v>
+      </c>
+      <c r="C107" t="s">
         <v>263</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="E107" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="E107" s="12" t="s">
-        <v>266</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>9</v>
@@ -3478,162 +3468,162 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="15" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="17" t="s">
+    <row r="3">
+      <c r="A3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="D3" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="17" t="s">
+    <row r="9" ht="14.25">
+      <c r="A9" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="D9" s="17" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17" t="s">
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="15" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="15"/>
     </row>
   </sheetData>
   <sortState ref="A2:D10" columnSort="0">

</xml_diff>

<commit_message>
add: EU taxon list
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -11,6 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Traits!$A$1:$F$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Traits!$A$1:$F$138</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
@@ -265,9 +266,6 @@
     <t>0,1</t>
   </si>
   <si>
-    <t>logical</t>
-  </si>
-  <si>
     <t>Chamaephyte</t>
   </si>
   <si>
@@ -544,517 +542,520 @@
     <t>PV.butterflies</t>
   </si>
   <si>
+    <t>Dcube</t>
+  </si>
+  <si>
+    <t>fruit_type</t>
+  </si>
+  <si>
+    <t>fruit.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the ecological characteristics of the fruit that are related to seed dispersal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 classes</t>
+  </si>
+  <si>
+    <t>dia_type</t>
+  </si>
+  <si>
+    <t>dia.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the morphological structure that acts as the diaspore, i.e. the diasporsal unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 classes</t>
+  </si>
+  <si>
+    <t>dia_exposure</t>
+  </si>
+  <si>
+    <t>dia.exposure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diaspore exposure, accessibility of dispersal vectors to the diaspores within the infructescence;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 classes</t>
+  </si>
+  <si>
+    <t>dia_hetero</t>
+  </si>
+  <si>
+    <t>dia.hetero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heterodiaspory, a heterodiaspore species features more than one diaspore type</t>
+  </si>
+  <si>
+    <t>(0,1)</t>
+  </si>
+  <si>
+    <t>dia_app_nutrient</t>
+  </si>
+  <si>
+    <t>dia.app.nutrient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrients, indicator for dysochory and endozoochory</t>
+  </si>
+  <si>
+    <t>dia_app_elon</t>
+  </si>
+  <si>
+    <t>dia.app.elon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elongated appendages, indicator for anemochory and epizoocccchory</t>
+  </si>
+  <si>
+    <t>dia_app_hook</t>
+  </si>
+  <si>
+    <t>dia.app.hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hooked appendages, indicator for epizoochory</t>
+  </si>
+  <si>
+    <t>dia_app_muci</t>
+  </si>
+  <si>
+    <t>dia.app.muci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mucilaginous surface, indicator for epizoochory and endozoochory</t>
+  </si>
+  <si>
+    <t>dia_mass</t>
+  </si>
+  <si>
+    <t>dia.mass.mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore mass, weight of one diaspore including all appendages</t>
+  </si>
+  <si>
+    <t>dia_surfacestructure</t>
+  </si>
+  <si>
+    <t>dia.surfacestructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore surface structure, smoothness of a diaspore's surface based on images of the diaspores. very smooth surface =1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score (0-1)</t>
+  </si>
+  <si>
+    <t>dia_length</t>
+  </si>
+  <si>
+    <t>dia.length.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore length, i.e. the longest axis including all appendages</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>dia_width</t>
+  </si>
+  <si>
+    <t>dia.width.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore width, i.e. the second longest axis perpendicular to length, including all appendages</t>
+  </si>
+  <si>
+    <t>dia_height</t>
+  </si>
+  <si>
+    <t>dia.height.mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore height, i.e. the shortest axis perpendicular to length and width, including all appendages</t>
+  </si>
+  <si>
+    <t>dia_shape</t>
+  </si>
+  <si>
+    <t>dia.shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore shape, deviation of a diaspore's shape from a sphere in three dimension; sphere =0</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>dia_form</t>
+  </si>
+  <si>
+    <t>dia.form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore form, form of diaspore in categories</t>
+  </si>
+  <si>
+    <t>vterm</t>
+  </si>
+  <si>
+    <t>term.velocity.m.s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminal velocity, maximum speed of a failing diaspore in still air</t>
+  </si>
+  <si>
+    <t>m.s-1</t>
+  </si>
+  <si>
+    <t>rank_ane</t>
+  </si>
+  <si>
+    <t>rank.ane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anemochory ranking index, assess how well a species is adapted to anemochory (wind dispersal)</t>
+  </si>
+  <si>
+    <t>rank_hydro</t>
+  </si>
+  <si>
+    <t>rank.hydro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrochory ranking index, assess how well a species is adapted to hydrochory (water dispersal)</t>
+  </si>
+  <si>
+    <t>rank_epi_wool</t>
+  </si>
+  <si>
+    <t>rank.epi.wool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epizoochory ranking index, assess how well a species is adapted to epizoochory (external animal dispersal)</t>
+  </si>
+  <si>
+    <t>diaspore_seeds_class</t>
+  </si>
+  <si>
+    <t>diaspore.seeds.class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaspore seed class</t>
+  </si>
+  <si>
+    <t>Hodgson2023</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>SLA.mm2.mg-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific leaf area</t>
+  </si>
+  <si>
+    <t>mm2.mg-1</t>
+  </si>
+  <si>
+    <t>ARNODE</t>
+  </si>
+  <si>
+    <t>Arnode.mm2.mm-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area per node/thickness</t>
+  </si>
+  <si>
+    <t>mm2.mm-1</t>
+  </si>
+  <si>
+    <t>LOGCANH</t>
+  </si>
+  <si>
+    <t>Log2.canopy.height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy height (converted to log2 bins)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log 2 bins cm</t>
+  </si>
+  <si>
+    <t>LOGCAND</t>
+  </si>
+  <si>
+    <t>Log2.canopy.diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy diameter (converted to log2 bins)</t>
+  </si>
+  <si>
+    <t>VEGPROP</t>
+  </si>
+  <si>
+    <t>Vegprop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetative propagation  of perennials</t>
+  </si>
+  <si>
+    <t>LIFEHIST</t>
+  </si>
+  <si>
+    <t>Lifehist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annual, herbaceous perennial, wood perennial, biennial</t>
+  </si>
+  <si>
+    <t>GIFT</t>
+  </si>
+  <si>
+    <t>Growth_form_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herb, shrub, tree, other</t>
+  </si>
+  <si>
+    <t>Lifecycle_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annual, biennial, perennial, variable</t>
+  </si>
+  <si>
+    <t>Growth_form_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herb, graminoid, forb, subshrub, shrub, tree, palm, other</t>
+  </si>
+  <si>
+    <t>Plant_height_max</t>
+  </si>
+  <si>
+    <t>Plant_height_max_m</t>
+  </si>
+  <si>
+    <t>Plant_height_min</t>
+  </si>
+  <si>
+    <t>Plant_height_min_m</t>
+  </si>
+  <si>
+    <t>Photosynthetic_pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3, C4, CAM</t>
+  </si>
+  <si>
+    <t>Seed_mass_mean</t>
+  </si>
+  <si>
+    <t>Seed_mass_mean_g</t>
+  </si>
+  <si>
+    <t>Plant_height_mean</t>
+  </si>
+  <si>
+    <t>Plant_height_mean_m</t>
+  </si>
+  <si>
+    <t>Seed_mass_min</t>
+  </si>
+  <si>
+    <t>Seed_mass_min_g</t>
+  </si>
+  <si>
+    <t>Seed_mass_max</t>
+  </si>
+  <si>
+    <t>Seed_mass_max_g</t>
+  </si>
+  <si>
+    <t>Leaf_length_max</t>
+  </si>
+  <si>
+    <t>Leaf_length_max_cm</t>
+  </si>
+  <si>
+    <t>Leaf_width_max</t>
+  </si>
+  <si>
+    <t>Leaf_width_max_cm</t>
+  </si>
+  <si>
+    <t>Leaf_width_min</t>
+  </si>
+  <si>
+    <t>Leaf_width_min_cm</t>
+  </si>
+  <si>
+    <t>Leaf_length_min</t>
+  </si>
+  <si>
+    <t>Leaf_length_min_cm</t>
+  </si>
+  <si>
+    <t>Leaf_length_mean</t>
+  </si>
+  <si>
+    <t>Leaf_length_mean_cm</t>
+  </si>
+  <si>
+    <t>Dispersal_syndrome_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anemochorous, zoochorous, autochorous, hydrochorous, unspecialized</t>
+  </si>
+  <si>
+    <t>Leaf_width_mean</t>
+  </si>
+  <si>
+    <t>Leaf_width_mean_cm</t>
+  </si>
+  <si>
+    <t>Dispersal_syndrome_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anemochorous, anthropochorous, autochorous, endozoochorous, epizoochorous, hydrochorous, myrmecochorous, unspecialized, zoochorous</t>
+  </si>
+  <si>
+    <t>Pollination_syndrome_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biotic, abiotic</t>
+  </si>
+  <si>
+    <t>Pollination_syndrome_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind, water, insect, bird, bat, other</t>
+  </si>
+  <si>
+    <t>Pollination_syndrome_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind, water, bee, beetle, ant, butterfly, moth, fly, insect, bird, bat, other</t>
+  </si>
+  <si>
+    <t>Inflorescence_length_max</t>
+  </si>
+  <si>
+    <t>Inflorescence_length_max_m</t>
+  </si>
+  <si>
+    <t>Inflorescence_length_min</t>
+  </si>
+  <si>
+    <t>Inflorescence_length_min_m</t>
+  </si>
+  <si>
+    <t>Fruit_colour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red, pink, blue, yellow, orange, green, white, violet, black, grey, brown, other</t>
+  </si>
+  <si>
+    <t>Flower_length_max</t>
+  </si>
+  <si>
+    <t>Flower_length_max_cm</t>
+  </si>
+  <si>
+    <t>Flower_colour</t>
+  </si>
+  <si>
+    <t>Flower_length_min</t>
+  </si>
+  <si>
+    <t>Flower_length_min_cm</t>
+  </si>
+  <si>
+    <t>Leaf_size_mean</t>
+  </si>
+  <si>
+    <t>Leaf_size_mean_cm2</t>
+  </si>
+  <si>
+    <t>cm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raceme, corymb, umbel, panicle, corymbose_panicle, spike, catkin, pseudoraceme, cyme, fascicle</t>
+  </si>
+  <si>
+    <t>categorial</t>
+  </si>
+  <si>
+    <t>Flower_width_max</t>
+  </si>
+  <si>
+    <t>Flower_width_max_cm</t>
+  </si>
+  <si>
+    <t>Flower_width_min</t>
+  </si>
+  <si>
+    <t>Flower_width_min_cm</t>
+  </si>
+  <si>
+    <t>SLA_mean</t>
+  </si>
+  <si>
+    <t>SLA_mean_cm2.g-1</t>
+  </si>
+  <si>
+    <t>cm²/g</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>At_Vinedivers</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>At_Fr_Ro_Sp_Species_List_VINEDIVERS.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julve, Ph., 2024 ff. - Baseflor. Index botanique, écologique et chorologique de la flore de France. Version : 01 juin 2024. https://www.tela-botanica.org/projets/phytosociologie</t>
+  </si>
+  <si>
+    <t>https://www.tela-botanica.org/projets/phytosociologie/porte-documents/</t>
+  </si>
+  <si>
+    <t>CATMINAT/baseflor.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enquist BJ, Condit R, Peet RK, Schildhauer M, Thiers BM. (2016) Cyberinfrastructure for an integrated botanical information network to investigate the ecological impacts of global climate change on plant biodiversity. PeerJ Preprints 4:e2615v2</t>
+  </si>
+  <si>
+    <t>https://bien.nceas.ucsb.edu/bien/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">access via API</t>
+  </si>
+  <si>
     <t>dcube</t>
-  </si>
-  <si>
-    <t>fruit_type</t>
-  </si>
-  <si>
-    <t>fruit.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of the ecological characteristics of the fruit that are related to seed dispersal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 classes</t>
-  </si>
-  <si>
-    <t>dia_type</t>
-  </si>
-  <si>
-    <t>dia.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of the morphological structure that acts as the diaspore, i.e. the diasporsal unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 classes</t>
-  </si>
-  <si>
-    <t>dia_exposure</t>
-  </si>
-  <si>
-    <t>dia.exposure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diaspore exposure, accessibility of dispersal vectors to the diaspores within the infructescence;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 classes</t>
-  </si>
-  <si>
-    <t>dia_hetero</t>
-  </si>
-  <si>
-    <t>dia.hetero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heterodiaspory, a heterodiaspore species features more than one diaspore type</t>
-  </si>
-  <si>
-    <t>(0,1)</t>
-  </si>
-  <si>
-    <t>dia_app_nutrient</t>
-  </si>
-  <si>
-    <t>dia.app.nutrient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrients, indicator for dysochory and endozoochory</t>
-  </si>
-  <si>
-    <t>dia_app_elon</t>
-  </si>
-  <si>
-    <t>dia.app.elon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elongated appendages, indicator for anemochory and epizoocccchory</t>
-  </si>
-  <si>
-    <t>dia_app_hook</t>
-  </si>
-  <si>
-    <t>dia.app.hook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hooked appendages, indicator for epizoochory</t>
-  </si>
-  <si>
-    <t>dia_app_muci</t>
-  </si>
-  <si>
-    <t>dia.app.muci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mucilaginous surface, indicator for epizoochory and endozoochory</t>
-  </si>
-  <si>
-    <t>dia_mass</t>
-  </si>
-  <si>
-    <t>dia.mass.mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore mass, weight of one diaspore including all appendages</t>
-  </si>
-  <si>
-    <t>dia_surfacestructure</t>
-  </si>
-  <si>
-    <t>dia.surfacestructure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore surface structure, smoothness of a diaspore's surface based on images of the diaspores. very smooth surface =1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score (0-1)</t>
-  </si>
-  <si>
-    <t>dia_length</t>
-  </si>
-  <si>
-    <t>dia.length.mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore length, i.e. the longest axis including all appendages</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>dia_width</t>
-  </si>
-  <si>
-    <t>dia.width.mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore width, i.e. the second longest axis perpendicular to length, including all appendages</t>
-  </si>
-  <si>
-    <t>dia_height</t>
-  </si>
-  <si>
-    <t>dia.height.mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore height, i.e. the shortest axis perpendicular to length and width, including all appendages</t>
-  </si>
-  <si>
-    <t>dia_shape</t>
-  </si>
-  <si>
-    <t>dia.shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore shape, deviation of a diaspore's shape from a sphere in three dimension; sphere =0</t>
-  </si>
-  <si>
-    <t>ratio</t>
-  </si>
-  <si>
-    <t>dia_form</t>
-  </si>
-  <si>
-    <t>dia.form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore form, form of diaspore in categories</t>
-  </si>
-  <si>
-    <t>vterm</t>
-  </si>
-  <si>
-    <t>term.velocity.m.s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">terminal velocity, maximum speed of a failing diaspore in still air</t>
-  </si>
-  <si>
-    <t>m.s-1</t>
-  </si>
-  <si>
-    <t>rank_ane</t>
-  </si>
-  <si>
-    <t>rank.ane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anemochory ranking index, assess how well a species is adapted to anemochory (wind dispersal)</t>
-  </si>
-  <si>
-    <t>rank_hydro</t>
-  </si>
-  <si>
-    <t>rank.hydro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrochory ranking index, assess how well a species is adapted to hydrochory (water dispersal)</t>
-  </si>
-  <si>
-    <t>rank_epi_wool</t>
-  </si>
-  <si>
-    <t>rank.epi.wool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epizoochory ranking index, assess how well a species is adapted to epizoochory (external animal dispersal)</t>
-  </si>
-  <si>
-    <t>diaspore_seeds_class</t>
-  </si>
-  <si>
-    <t>diaspore.seeds.class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diaspore seed class</t>
-  </si>
-  <si>
-    <t>Hodgson2023</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>SLA.mm2.mg-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific leaf area</t>
-  </si>
-  <si>
-    <t>mm2.mg-1</t>
-  </si>
-  <si>
-    <t>ARNODE</t>
-  </si>
-  <si>
-    <t>Arnode.mm2.mm-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area per node/thickness</t>
-  </si>
-  <si>
-    <t>mm2.mm-1</t>
-  </si>
-  <si>
-    <t>LOGCANH</t>
-  </si>
-  <si>
-    <t>Log2.canopy.height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canopy height (converted to log2 bins)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log 2 bins cm</t>
-  </si>
-  <si>
-    <t>LOGCAND</t>
-  </si>
-  <si>
-    <t>Log2.canopy.diameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canopy diameter (converted to log2 bins)</t>
-  </si>
-  <si>
-    <t>VEGPROP</t>
-  </si>
-  <si>
-    <t>Vegprop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vegetative propagation  of perennials</t>
-  </si>
-  <si>
-    <t>LIFEHIST</t>
-  </si>
-  <si>
-    <t>Lifehist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annual, herbaceous perennial, wood perennial, biennial</t>
-  </si>
-  <si>
-    <t>GIFT</t>
-  </si>
-  <si>
-    <t>Growth_form_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herb, shrub, tree, other</t>
-  </si>
-  <si>
-    <t>Lifecycle_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annual, biennial, perennial, variable</t>
-  </si>
-  <si>
-    <t>Growth_form_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herb, graminoid, forb, subshrub, shrub, tree, palm, other</t>
-  </si>
-  <si>
-    <t>Plant_height_max</t>
-  </si>
-  <si>
-    <t>Plant_height_max_m</t>
-  </si>
-  <si>
-    <t>Plant_height_min</t>
-  </si>
-  <si>
-    <t>Plant_height_min_m</t>
-  </si>
-  <si>
-    <t>Photosynthetic_pathway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3, C4, CAM</t>
-  </si>
-  <si>
-    <t>Seed_mass_mean</t>
-  </si>
-  <si>
-    <t>Seed_mass_mean_g</t>
-  </si>
-  <si>
-    <t>Plant_height_mean</t>
-  </si>
-  <si>
-    <t>Plant_height_mean_m</t>
-  </si>
-  <si>
-    <t>Seed_mass_min</t>
-  </si>
-  <si>
-    <t>Seed_mass_min_g</t>
-  </si>
-  <si>
-    <t>Seed_mass_max</t>
-  </si>
-  <si>
-    <t>Seed_mass_max_g</t>
-  </si>
-  <si>
-    <t>Leaf_length_max</t>
-  </si>
-  <si>
-    <t>Leaf_length_max_cm</t>
-  </si>
-  <si>
-    <t>Leaf_width_max</t>
-  </si>
-  <si>
-    <t>Leaf_width_max_cm</t>
-  </si>
-  <si>
-    <t>Leaf_width_min</t>
-  </si>
-  <si>
-    <t>Leaf_width_min_cm</t>
-  </si>
-  <si>
-    <t>Leaf_length_min</t>
-  </si>
-  <si>
-    <t>Leaf_length_min_cm</t>
-  </si>
-  <si>
-    <t>Leaf_length_mean</t>
-  </si>
-  <si>
-    <t>Leaf_length_mean_cm</t>
-  </si>
-  <si>
-    <t>Dispersal_syndrome_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anemochorous, zoochorous, autochorous, hydrochorous, unspecialized</t>
-  </si>
-  <si>
-    <t>Leaf_width_mean</t>
-  </si>
-  <si>
-    <t>Leaf_width_mean_cm</t>
-  </si>
-  <si>
-    <t>Dispersal_syndrome_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anemochorous, anthropochorous, autochorous, endozoochorous, epizoochorous, hydrochorous, myrmecochorous, unspecialized, zoochorous</t>
-  </si>
-  <si>
-    <t>Pollination_syndrome_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biotic, abiotic</t>
-  </si>
-  <si>
-    <t>Pollination_syndrome_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind, water, insect, bird, bat, other</t>
-  </si>
-  <si>
-    <t>Pollination_syndrome_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind, water, bee, beetle, ant, butterfly, moth, fly, insect, bird, bat, other</t>
-  </si>
-  <si>
-    <t>Inflorescence_length_max</t>
-  </si>
-  <si>
-    <t>Inflorescence_length_max_m</t>
-  </si>
-  <si>
-    <t>Inflorescence_length_min</t>
-  </si>
-  <si>
-    <t>Inflorescence_length_min_m</t>
-  </si>
-  <si>
-    <t>Fruit_colour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red, pink, blue, yellow, orange, green, white, violet, black, grey, brown, other</t>
-  </si>
-  <si>
-    <t>Flower_length_max</t>
-  </si>
-  <si>
-    <t>Flower_length_max_cm</t>
-  </si>
-  <si>
-    <t>Flower_colour</t>
-  </si>
-  <si>
-    <t>Flower_length_min</t>
-  </si>
-  <si>
-    <t>Flower_length_min_cm</t>
-  </si>
-  <si>
-    <t>Leaf_size_mean</t>
-  </si>
-  <si>
-    <t>Leaf_size_mean_cm2</t>
-  </si>
-  <si>
-    <t>cm²</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raceme, corymb, umbel, panicle, corymbose_panicle, spike, catkin, pseudoraceme, cyme, fascicle</t>
-  </si>
-  <si>
-    <t>categorial</t>
-  </si>
-  <si>
-    <t>Flower_width_max</t>
-  </si>
-  <si>
-    <t>Flower_width_max_cm</t>
-  </si>
-  <si>
-    <t>Flower_width_min</t>
-  </si>
-  <si>
-    <t>Flower_width_min_cm</t>
-  </si>
-  <si>
-    <t>SLA_mean</t>
-  </si>
-  <si>
-    <t>SLA_mean_cm2.g-1</t>
-  </si>
-  <si>
-    <t>cm²/g</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>At_Vinedivers</t>
-  </si>
-  <si>
-    <t>private</t>
-  </si>
-  <si>
-    <t>At_Fr_Ro_Sp_Species_List_VINEDIVERS.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julve, Ph., 2024 ff. - Baseflor. Index botanique, écologique et chorologique de la flore de France. Version : 01 juin 2024. https://www.tela-botanica.org/projets/phytosociologie</t>
-  </si>
-  <si>
-    <t>https://www.tela-botanica.org/projets/phytosociologie/porte-documents/</t>
-  </si>
-  <si>
-    <t>CATMINAT/baseflor.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enquist BJ, Condit R, Peet RK, Schildhauer M, Thiers BM. (2016) Cyberinfrastructure for an integrated botanical information network to investigate the ecological impacts of global climate change on plant biodiversity. PeerJ Preprints 4:e2615v2</t>
-  </si>
-  <si>
-    <t>https://bien.nceas.ucsb.edu/bien/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">access via API</t>
   </si>
   <si>
     <t xml:space="preserve">Hintze, C., Heydel, F., Hoppe, C., Cunze, S., König, A., &amp; Tackenberg, O. (2013). D3: the dispersal and diaspore database–baseline data and statistics on seed dispersal. Perspectives in Plant Ecology, Evolution and Systematics, 15(3), 180-192.</t>
@@ -1305,7 +1306,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1314,13 +1315,13 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1330,9 +1331,6 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1859,7 +1857,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C100" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1902,8 +1900,8 @@
         <v>8</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1917,9 +1915,9 @@
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1933,9 +1931,9 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1980,7 +1978,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1995,7 +1993,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2006,10 +2004,10 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2020,10 +2018,10 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2034,10 +2032,10 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2065,7 +2063,7 @@
       <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2076,7 +2074,7 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F14" t="s">
@@ -2093,7 +2091,7 @@
       <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2104,10 +2102,10 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2118,10 +2116,10 @@
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2132,10 +2130,10 @@
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2146,10 +2144,10 @@
       <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2160,10 +2158,10 @@
       <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2174,10 +2172,10 @@
       <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2188,10 +2186,10 @@
       <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2202,10 +2200,10 @@
       <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2216,233 +2214,233 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C34" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C38" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2459,8 +2457,8 @@
       <c r="E39" t="s">
         <v>80</v>
       </c>
-      <c r="F39" t="s">
-        <v>81</v>
+      <c r="F39" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="40" ht="14.25">
@@ -2468,16 +2466,16 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E40" t="s">
         <v>80</v>
       </c>
-      <c r="F40" t="s">
-        <v>81</v>
+      <c r="F40" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="41" ht="14.25">
@@ -2485,16 +2483,16 @@
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E41" t="s">
         <v>80</v>
       </c>
-      <c r="F41" t="s">
-        <v>81</v>
+      <c r="F41" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="42" ht="14.25">
@@ -2502,16 +2500,16 @@
         <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E42" t="s">
         <v>80</v>
       </c>
-      <c r="F42" t="s">
-        <v>81</v>
+      <c r="F42" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="43" ht="14.25">
@@ -2519,16 +2517,16 @@
         <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="E43" t="s">
         <v>80</v>
       </c>
-      <c r="F43" t="s">
-        <v>81</v>
+      <c r="F43" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="44" ht="14.25">
@@ -2536,16 +2534,16 @@
         <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E44" t="s">
         <v>80</v>
       </c>
-      <c r="F44" t="s">
-        <v>81</v>
+      <c r="F44" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="45" ht="14.25">
@@ -2553,661 +2551,661 @@
         <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E45" t="s">
         <v>80</v>
       </c>
-      <c r="F45" t="s">
-        <v>81</v>
+      <c r="F45" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>89</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>90</v>
-      </c>
-      <c r="D46" t="s">
-        <v>91</v>
       </c>
       <c r="E46" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" t="s">
         <v>93</v>
-      </c>
-      <c r="D47" t="s">
-        <v>94</v>
       </c>
       <c r="E47" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="E49" t="s">
         <v>98</v>
       </c>
-      <c r="E49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" ht="28.5">
       <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="C50" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" ht="28.5">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" ht="28.5">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" t="s">
         <v>106</v>
       </c>
-      <c r="E52" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="53" ht="14.25">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="E53" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="54" ht="28.5">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>111</v>
-      </c>
       <c r="E54" t="s">
-        <v>107</v>
-      </c>
-      <c r="F54" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="55" ht="14.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F55" s="7" t="s">
+      <c r="F55" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B56" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" t="s">
         <v>117</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" s="2"/>
+      <c r="E57" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" ht="14.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F58" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" ht="14.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="F60" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" ht="14.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="F62" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" ht="14.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" ht="15">
       <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" t="s">
         <v>130</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>131</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="E64" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" ht="15">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
         <v>135</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>136</v>
-      </c>
-      <c r="D65" t="s">
-        <v>137</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" ht="15">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
         <v>138</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>139</v>
-      </c>
-      <c r="D66" t="s">
-        <v>140</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="67" ht="15">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" t="s">
         <v>141</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>142</v>
       </c>
-      <c r="D67" t="s">
-        <v>143</v>
-      </c>
       <c r="E67" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F67" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="68" ht="15">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" t="s">
         <v>144</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="E68" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F68" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F68" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="69" ht="15">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" t="s">
         <v>147</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="E69" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E69" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" t="s">
         <v>151</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="F70" s="7" t="s">
+      <c r="D70" s="2"/>
+      <c r="F70" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F71" s="7" t="s">
+      <c r="F71" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F72" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F72" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="E73" t="s">
         <v>31</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="E74" t="s">
         <v>31</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="75" ht="14.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="F75" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F75" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
+        <v>161</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F77" s="7" t="s">
+      <c r="F77" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F78" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F79" s="7" t="s">
+      <c r="F79" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="80" ht="14.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="E80" t="s">
         <v>31</v>
       </c>
-      <c r="F80" s="7" t="s">
+      <c r="F80" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C81" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E81" s="6" t="s">
+      <c r="E81" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="82" ht="14.25">
       <c r="A82" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" t="s">
         <v>174</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="D82" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="E82" t="s">
         <v>177</v>
       </c>
-      <c r="E82" t="s">
-        <v>178</v>
-      </c>
-      <c r="F82" s="6" t="s">
+      <c r="F82" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="D83" t="s">
         <v>180</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>181</v>
-      </c>
-      <c r="E83" t="s">
-        <v>182</v>
       </c>
       <c r="F83" t="s">
         <v>9</v>
@@ -3215,160 +3213,160 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="D84" t="s">
         <v>184</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>185</v>
       </c>
-      <c r="E84" t="s">
-        <v>186</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" s="6"/>
+      <c r="F84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="2"/>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="D85" t="s">
         <v>188</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>189</v>
       </c>
-      <c r="E85" t="s">
-        <v>190</v>
-      </c>
-      <c r="F85" t="s">
-        <v>81</v>
+      <c r="F85" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="D86" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D86" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F86" t="s">
-        <v>81</v>
+      <c r="E86" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="D87" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D87" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>81</v>
+      <c r="E87" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="88" ht="14.25">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
+        <v>196</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="D88" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>81</v>
+      <c r="E88" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B89" t="s">
+        <v>199</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="D89" t="s">
         <v>201</v>
       </c>
-      <c r="D89" t="s">
-        <v>202</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>81</v>
+      <c r="E89" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B90" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="D90" t="s">
         <v>204</v>
-      </c>
-      <c r="D90" t="s">
-        <v>205</v>
       </c>
       <c r="E90" t="s">
         <v>73</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F90" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B91" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="D91" t="s">
         <v>207</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>208</v>
-      </c>
-      <c r="E91" t="s">
-        <v>209</v>
       </c>
       <c r="F91" t="s">
         <v>59</v>
@@ -3376,59 +3374,59 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B92" t="s">
+        <v>209</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="D92" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="E92" t="s">
         <v>212</v>
       </c>
-      <c r="E92" t="s">
-        <v>213</v>
-      </c>
-      <c r="F92" s="7" t="s">
+      <c r="F92" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B93" t="s">
+        <v>213</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="D93" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D93" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="E93" t="s">
-        <v>213</v>
-      </c>
-      <c r="F93" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F93" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="94" ht="14.25">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="D94" t="s">
         <v>218</v>
       </c>
-      <c r="D94" t="s">
-        <v>219</v>
-      </c>
       <c r="E94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F94" t="s">
         <v>59</v>
@@ -3436,19 +3434,19 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" t="s">
+        <v>219</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="D95" t="s">
         <v>221</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>222</v>
-      </c>
-      <c r="E95" t="s">
-        <v>223</v>
       </c>
       <c r="F95" t="s">
         <v>59</v>
@@ -3456,19 +3454,19 @@
     </row>
     <row r="96" ht="14.25">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B96" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="D96" t="s">
         <v>225</v>
       </c>
-      <c r="D96" t="s">
-        <v>226</v>
-      </c>
       <c r="E96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F96" t="s">
         <v>9</v>
@@ -3476,19 +3474,19 @@
     </row>
     <row r="97" ht="14.25">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="D97" t="s">
         <v>228</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>229</v>
-      </c>
-      <c r="E97" t="s">
-        <v>230</v>
       </c>
       <c r="F97" t="s">
         <v>59</v>
@@ -3496,19 +3494,19 @@
     </row>
     <row r="98" ht="14.25">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="D98" t="s">
         <v>232</v>
       </c>
-      <c r="D98" t="s">
-        <v>233</v>
-      </c>
       <c r="E98" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F98" t="s">
         <v>59</v>
@@ -3516,19 +3514,19 @@
     </row>
     <row r="99" ht="14.25">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B99" t="s">
+        <v>233</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="D99" t="s">
         <v>235</v>
       </c>
-      <c r="D99" t="s">
-        <v>236</v>
-      </c>
       <c r="E99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F99" t="s">
         <v>59</v>
@@ -3536,19 +3534,19 @@
     </row>
     <row r="100" ht="14.25">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="D100" t="s">
         <v>238</v>
       </c>
-      <c r="D100" t="s">
-        <v>239</v>
-      </c>
       <c r="E100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F100" t="s">
         <v>59</v>
@@ -3556,682 +3554,682 @@
     </row>
     <row r="101" ht="14.25">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
+        <v>239</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="D101" t="s">
         <v>241</v>
       </c>
-      <c r="D101" t="s">
-        <v>242</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>59</v>
+      <c r="F101" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" t="s">
+        <v>242</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="C102" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="D102" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="E102" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="E102" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="F102" s="7" t="s">
+      <c r="F102" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="103" ht="14.25">
       <c r="A103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B103" t="s">
+        <v>247</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="D103" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="E103" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="E103" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="F103" s="7" t="s">
+      <c r="F103" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B104" t="s">
+        <v>251</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="D104" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="E104" t="s">
         <v>254</v>
       </c>
-      <c r="E104" t="s">
-        <v>255</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>59</v>
+      <c r="F104" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="105" ht="14.25">
       <c r="A105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B105" t="s">
+        <v>255</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="D105" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="E105" t="s">
-        <v>255</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>59</v>
+        <v>254</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B106" t="s">
+        <v>258</v>
+      </c>
+      <c r="C106" t="s">
         <v>259</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>81</v>
+      <c r="E106" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B107" t="s">
+        <v>261</v>
+      </c>
+      <c r="C107" t="s">
         <v>262</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="E107" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="E107" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="F107" s="7" t="s">
+      <c r="F107" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" t="s">
+        <v>265</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="C108" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E108" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="F108" s="7" t="s">
+      <c r="F108" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" t="s">
-        <v>266</v>
-      </c>
-      <c r="B109" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C109" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="F109" s="7" t="s">
+      <c r="F109" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" t="s">
-        <v>266</v>
-      </c>
-      <c r="B110" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E110" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C110" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="F110" s="7" t="s">
+      <c r="F110" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C111" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C111" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E111" s="7" t="s">
+      <c r="E111" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F111" s="7" t="s">
+      <c r="F111" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" t="s">
-        <v>266</v>
-      </c>
-      <c r="B112" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C112" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="E112" s="7" t="s">
+      <c r="E112" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F112" s="7" t="s">
+      <c r="F112" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" t="s">
-        <v>266</v>
-      </c>
-      <c r="B113" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E113" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F113" s="7" t="s">
+      <c r="F113" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" t="s">
-        <v>266</v>
-      </c>
-      <c r="B114" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C114" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="C114" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="E114" s="7" t="s">
+      <c r="E114" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F114" s="7" t="s">
+      <c r="F114" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" t="s">
-        <v>266</v>
-      </c>
-      <c r="B115" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C115" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="C115" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="E115" s="7" t="s">
+      <c r="E115" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F115" s="7" t="s">
+      <c r="F115" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" t="s">
-        <v>266</v>
-      </c>
-      <c r="B116" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C116" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C116" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="E116" s="7" t="s">
+      <c r="E116" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F116" s="7" t="s">
+      <c r="F116" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" t="s">
-        <v>266</v>
-      </c>
-      <c r="B117" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C117" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C117" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E117" s="7" t="s">
+      <c r="E117" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F117" s="7" t="s">
+      <c r="F117" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" t="s">
-        <v>266</v>
-      </c>
-      <c r="B118" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C118" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F118" s="7" t="s">
+      <c r="E118" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F118" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" t="s">
-        <v>266</v>
-      </c>
-      <c r="B119" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C119" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="E119" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F119" s="7" t="s">
+      <c r="E119" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F119" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" t="s">
-        <v>266</v>
-      </c>
-      <c r="B120" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C120" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="E120" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F120" s="7" t="s">
+      <c r="E120" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F120" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" t="s">
-        <v>266</v>
-      </c>
-      <c r="B121" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C121" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F121" s="7" t="s">
+      <c r="E121" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F121" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" t="s">
-        <v>266</v>
-      </c>
-      <c r="B122" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C122" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="E122" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F122" s="7" t="s">
+      <c r="E122" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F122" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="123" ht="14.25">
       <c r="A123" t="s">
-        <v>266</v>
-      </c>
-      <c r="B123" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E123" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C123" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="F123" s="7" t="s">
+      <c r="F123" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="124" ht="14.25">
       <c r="A124" t="s">
-        <v>266</v>
-      </c>
-      <c r="B124" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C124" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="C124" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="E124" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F124" s="7" t="s">
+      <c r="E124" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F124" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="125" ht="14.25">
       <c r="A125" t="s">
-        <v>266</v>
-      </c>
-      <c r="B125" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E125" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C125" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E125" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="F125" s="7" t="s">
+      <c r="F125" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" t="s">
-        <v>266</v>
-      </c>
-      <c r="B126" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E126" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C126" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="F126" s="7" t="s">
+      <c r="F126" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" t="s">
-        <v>266</v>
-      </c>
-      <c r="B127" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E127" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C127" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="F127" s="7" t="s">
+      <c r="F127" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="128" ht="14.25">
       <c r="A128" t="s">
-        <v>266</v>
-      </c>
-      <c r="B128" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E128" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="E128" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="F128" s="7" t="s">
+      <c r="F128" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="129" ht="14.25">
       <c r="A129" t="s">
-        <v>266</v>
-      </c>
-      <c r="B129" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C129" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="C129" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="E129" s="7" t="s">
+      <c r="E129" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F129" s="7" t="s">
+      <c r="F129" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="130" ht="14.25">
       <c r="A130" t="s">
-        <v>266</v>
-      </c>
-      <c r="B130" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C130" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="E130" s="7" t="s">
+      <c r="E130" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F130" s="7" t="s">
+      <c r="F130" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="131" ht="14.25">
       <c r="A131" t="s">
-        <v>266</v>
-      </c>
-      <c r="B131" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E131" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="C131" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="F131" s="7" t="s">
+      <c r="F131" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="132" ht="14.25">
       <c r="A132" t="s">
-        <v>266</v>
-      </c>
-      <c r="B132" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C132" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="C132" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="E132" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F132" s="7" t="s">
+      <c r="E132" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F132" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="133" ht="14.25">
       <c r="A133" t="s">
-        <v>266</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="E133" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="F133" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F133" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="134" ht="14.25">
       <c r="A134" t="s">
-        <v>266</v>
-      </c>
-      <c r="B134" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C134" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C134" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="E134" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F134" s="7" t="s">
+      <c r="E134" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F134" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="135" ht="14.25">
       <c r="A135" t="s">
-        <v>266</v>
-      </c>
-      <c r="B135" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C135" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C135" s="13" t="s">
+      <c r="E135" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="E135" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="F135" s="7" t="s">
+      <c r="F135" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="136" ht="14.25">
       <c r="A136" t="s">
-        <v>266</v>
-      </c>
-      <c r="B136" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B136" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C136" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E136" s="7" t="s">
+      <c r="E136" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F136" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="F136" s="7" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="137" ht="14.25">
       <c r="A137" t="s">
-        <v>266</v>
-      </c>
-      <c r="B137" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C137" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="E137" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F137" s="7" t="s">
+      <c r="E137" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F137" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="138" ht="14.25">
       <c r="A138" t="s">
-        <v>266</v>
-      </c>
-      <c r="B138" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C138" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="C138" s="13" t="s">
+      <c r="E138" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25">
+      <c r="A139" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B139" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E138" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="139" ht="14.25">
-      <c r="A139" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B139" s="7" t="s">
+      <c r="C139" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C139" s="13" t="s">
+      <c r="E139" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="E139" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="F139" s="7" t="s">
+      <c r="F139" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4262,101 +4260,101 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="15" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="15" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="16" t="s">
+      <c r="B2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="D2" s="17" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="D3" s="17" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="D4" s="17" t="s">
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="6" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" t="s">
         <v>352</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>353</v>
       </c>
       <c r="D7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -4366,7 +4364,7 @@
       <c r="B8" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>356</v>
       </c>
       <c r="D8" t="s">
@@ -4374,84 +4372,84 @@
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: handle long trait databases
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
   <si>
     <t>database</t>
   </si>
@@ -242,6 +242,9 @@
     <t>seed.mass.mg</t>
   </si>
   <si>
+    <t>Seed.mass_mg</t>
+  </si>
+  <si>
     <t>mg</t>
   </si>
   <si>
@@ -254,6 +257,9 @@
     <t>whole.plant.height.m</t>
   </si>
   <si>
+    <t>Plant.height_m</t>
+  </si>
+  <si>
     <t>whole.plant.woodiness</t>
   </si>
   <si>
@@ -290,18 +296,12 @@
     <t xml:space="preserve">Plant height (m)</t>
   </si>
   <si>
-    <t>Plant.height_m</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plant height</t>
   </si>
   <si>
     <t xml:space="preserve">Seed mass (mg)</t>
   </si>
   <si>
-    <t>Seed.mass_mg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Seed mass</t>
   </si>
   <si>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">Plant Height</t>
   </si>
   <si>
-    <t>Plant_Height</t>
+    <t>Plant.height_cm</t>
   </si>
   <si>
     <t>cm</t>
@@ -842,13 +842,13 @@
     <t>Plant_height_max</t>
   </si>
   <si>
-    <t>Plant_height_max_m</t>
+    <t>Plant.height.max_m</t>
   </si>
   <si>
     <t>Plant_height_min</t>
   </si>
   <si>
-    <t>Plant_height_min_m</t>
+    <t>Plant.height.min_m</t>
   </si>
   <si>
     <t>Photosynthetic_pathway</t>
@@ -860,15 +860,12 @@
     <t>Seed_mass_mean</t>
   </si>
   <si>
-    <t>Seed_mass_mean_g</t>
+    <t>Seed.mass_g</t>
   </si>
   <si>
     <t>Plant_height_mean</t>
   </si>
   <si>
-    <t>Plant_height_mean_m</t>
-  </si>
-  <si>
     <t>Seed_mass_min</t>
   </si>
   <si>
@@ -1014,6 +1011,137 @@
   </si>
   <si>
     <t>cm²/g</t>
+  </si>
+  <si>
+    <t>FlorealData</t>
+  </si>
+  <si>
+    <t>Coul</t>
+  </si>
+  <si>
+    <t>Flower_color</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Couleur dominante de la </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t>ﬂ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">eur </t>
+    </r>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Specialization_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grassland Community Specialization Index</t>
+  </si>
+  <si>
+    <t>FDV</t>
+  </si>
+  <si>
+    <t>Lifeform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forme de vie </t>
+  </si>
+  <si>
+    <t>TailMoy</t>
+  </si>
+  <si>
+    <t>Plant_Height_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taille des espèces non graminéennes </t>
+  </si>
+  <si>
+    <t>Biolflor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed dry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed length</t>
+  </si>
+  <si>
+    <t>Seed.length_mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower pollinator and type of reward</t>
+  </si>
+  <si>
+    <t>Flower.pollinator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower sex</t>
+  </si>
+  <si>
+    <t>Flower.sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower sex timing</t>
+  </si>
+  <si>
+    <t>Flower.sex.timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower UV light reflectance</t>
+  </si>
+  <si>
+    <t>Flower.UV.light.reflectance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant lifespan (longevity)</t>
+  </si>
+  <si>
+    <t>Plant.lifespan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species strategy type according to Grime</t>
+  </si>
+  <si>
+    <t>Ecoflora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant height vegetative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant reproductive phenology timing (flowering time)</t>
+  </si>
+  <si>
+    <t>Plant.flowering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root rooting depth</t>
+  </si>
+  <si>
+    <t>Root.depth_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root type, root architecture</t>
+  </si>
+  <si>
+    <t>Root.type</t>
   </si>
   <si>
     <t>Database</t>
@@ -1196,7 +1324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -1215,6 +1343,18 @@
     </font>
     <font>
       <sz val="12.000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -1262,7 +1402,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -1302,11 +1442,24 @@
         <color theme="9" tint="0.39997558519241921"/>
       </horizontal>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1321,7 +1474,6 @@
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1329,24 +1481,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1857,7 +2024,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A139" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2225,11 +2392,11 @@
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C25" t="s">
-        <v>56</v>
+      <c r="C25" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>9</v>
@@ -2375,11 +2542,11 @@
       <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C34" t="s">
-        <v>72</v>
+      <c r="C34" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>59</v>
@@ -2390,10 +2557,10 @@
         <v>55</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>9</v>
@@ -2404,10 +2571,10 @@
         <v>55</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>9</v>
@@ -2418,10 +2585,10 @@
         <v>55</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>69</v>
@@ -2435,10 +2602,10 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>9</v>
@@ -2446,16 +2613,16 @@
     </row>
     <row r="39" ht="14.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>9</v>
@@ -2463,16 +2630,16 @@
     </row>
     <row r="40" ht="14.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>9</v>
@@ -2480,16 +2647,16 @@
     </row>
     <row r="41" ht="14.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" t="s">
-        <v>80</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>9</v>
@@ -2497,16 +2664,16 @@
     </row>
     <row r="42" ht="14.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>9</v>
@@ -2514,16 +2681,16 @@
     </row>
     <row r="43" ht="14.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>9</v>
@@ -2531,16 +2698,16 @@
     </row>
     <row r="44" ht="14.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>9</v>
@@ -2548,16 +2715,16 @@
     </row>
     <row r="45" ht="14.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>9</v>
@@ -2565,16 +2732,16 @@
     </row>
     <row r="46" ht="14.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
         <v>69</v>
@@ -2585,19 +2752,19 @@
     </row>
     <row r="47" ht="14.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D47" t="s">
         <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>59</v>
@@ -2605,7 +2772,7 @@
     </row>
     <row r="48" ht="14.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
         <v>94</v>
@@ -2619,7 +2786,7 @@
     </row>
     <row r="49" ht="14.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B49" t="s">
         <v>96</v>
@@ -2638,13 +2805,13 @@
       <c r="A50" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
         <v>101</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -2655,13 +2822,13 @@
       <c r="A51" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F51" s="6" t="s">
@@ -2672,13 +2839,13 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="9" t="s">
         <v>105</v>
       </c>
       <c r="E52" t="s">
@@ -2692,13 +2859,13 @@
       <c r="A53" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>108</v>
       </c>
       <c r="E53" t="s">
@@ -2712,13 +2879,13 @@
       <c r="A54" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="9" t="s">
         <v>110</v>
       </c>
       <c r="E54" t="s">
@@ -2732,13 +2899,13 @@
       <c r="A55" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F55" s="6" t="s">
@@ -2749,13 +2916,13 @@
       <c r="A56" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="9" t="s">
         <v>114</v>
       </c>
       <c r="F56" s="6" t="s">
@@ -2769,7 +2936,7 @@
       <c r="B57" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="11" t="s">
         <v>117</v>
       </c>
       <c r="D57" s="2"/>
@@ -3021,7 +3188,7 @@
         <v>155</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>155</v>
+        <v>28</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>9</v>
@@ -3346,7 +3513,7 @@
         <v>204</v>
       </c>
       <c r="E90" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>59</v>
@@ -3747,7 +3914,7 @@
       <c r="B111" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C111" s="11" t="s">
         <v>273</v>
       </c>
       <c r="E111" s="6" t="s">
@@ -3764,7 +3931,7 @@
       <c r="B112" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="11" t="s">
         <v>275</v>
       </c>
       <c r="E112" s="6" t="s">
@@ -3798,7 +3965,7 @@
       <c r="B114" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="11" t="s">
         <v>279</v>
       </c>
       <c r="E114" s="6" t="s">
@@ -3815,8 +3982,8 @@
       <c r="B115" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C115" s="6" t="s">
-        <v>281</v>
+      <c r="C115" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>69</v>
@@ -3830,10 +3997,10 @@
         <v>265</v>
       </c>
       <c r="B116" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>64</v>
@@ -3847,10 +4014,10 @@
         <v>265</v>
       </c>
       <c r="B117" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C117" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="C117" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>64</v>
@@ -3864,10 +4031,10 @@
         <v>265</v>
       </c>
       <c r="B118" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C118" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>287</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>118</v>
@@ -3881,10 +4048,10 @@
         <v>265</v>
       </c>
       <c r="B119" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>118</v>
@@ -3898,10 +4065,10 @@
         <v>265</v>
       </c>
       <c r="B120" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>118</v>
@@ -3915,10 +4082,10 @@
         <v>265</v>
       </c>
       <c r="B121" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>118</v>
@@ -3932,10 +4099,10 @@
         <v>265</v>
       </c>
       <c r="B122" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>118</v>
@@ -3949,13 +4116,13 @@
         <v>265</v>
       </c>
       <c r="B123" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="E123" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>9</v>
@@ -3966,10 +4133,10 @@
         <v>265</v>
       </c>
       <c r="B124" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C124" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>299</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>118</v>
@@ -3983,13 +4150,13 @@
         <v>265</v>
       </c>
       <c r="B125" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E125" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>9</v>
@@ -4000,13 +4167,13 @@
         <v>265</v>
       </c>
       <c r="B126" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E126" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E126" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>9</v>
@@ -4017,13 +4184,13 @@
         <v>265</v>
       </c>
       <c r="B127" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E127" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="E127" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="F127" s="6" t="s">
         <v>9</v>
@@ -4034,13 +4201,13 @@
         <v>265</v>
       </c>
       <c r="B128" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E128" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>9</v>
@@ -4051,10 +4218,10 @@
         <v>265</v>
       </c>
       <c r="B129" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C129" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>69</v>
@@ -4068,10 +4235,10 @@
         <v>265</v>
       </c>
       <c r="B130" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>69</v>
@@ -4085,13 +4252,13 @@
         <v>265</v>
       </c>
       <c r="B131" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E131" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>9</v>
@@ -4102,10 +4269,10 @@
         <v>265</v>
       </c>
       <c r="B132" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C132" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>118</v>
@@ -4119,13 +4286,13 @@
         <v>265</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F133" s="6" t="s">
         <v>9</v>
@@ -4136,10 +4303,10 @@
         <v>265</v>
       </c>
       <c r="B134" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C134" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>118</v>
@@ -4153,13 +4320,13 @@
         <v>265</v>
       </c>
       <c r="B135" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C135" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C135" s="6" t="s">
+      <c r="E135" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="E135" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="F135" s="6" t="s">
         <v>59</v>
@@ -4176,10 +4343,10 @@
         <v>18</v>
       </c>
       <c r="E136" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F136" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="F136" s="6" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="137" ht="14.25">
@@ -4187,10 +4354,10 @@
         <v>265</v>
       </c>
       <c r="B137" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>118</v>
@@ -4204,10 +4371,10 @@
         <v>265</v>
       </c>
       <c r="B138" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C138" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>118</v>
@@ -4221,23 +4388,326 @@
         <v>265</v>
       </c>
       <c r="B139" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C139" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C139" s="6" t="s">
+      <c r="E139" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="F139" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" ht="14.25">
+      <c r="A140" t="s">
         <v>330</v>
       </c>
-      <c r="F139" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="140" ht="14.25"/>
+      <c r="B140" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D140" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="141" ht="14.25">
+      <c r="A141" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D141" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" ht="14.25">
+      <c r="A142" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C142" t="s">
+        <v>338</v>
+      </c>
+      <c r="D142" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="143" ht="14.25">
+      <c r="A143" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C143" t="s">
+        <v>341</v>
+      </c>
+      <c r="D143" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E143" t="s">
+        <v>118</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" ht="14.25">
+      <c r="A144" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E144" t="s">
+        <v>74</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="145" ht="14.25">
+      <c r="A145" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="E145" t="s">
+        <v>212</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" ht="14.25">
+      <c r="A146" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" s="6"/>
+      <c r="F146" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="147" ht="14.25">
+      <c r="A147" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D147" s="6"/>
+      <c r="F147" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="148" ht="14.25">
+      <c r="A148" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="D148" s="6"/>
+      <c r="F148" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="149" ht="14.25">
+      <c r="A149" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D149" s="6"/>
+      <c r="F149" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="150" ht="14.25">
+      <c r="A150" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="D150" s="6"/>
+      <c r="F150" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" ht="14.25">
+      <c r="A151" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C151" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D151" s="6"/>
+      <c r="F151" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" ht="14.25">
+      <c r="A152" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" s="6"/>
+      <c r="F152" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="153" ht="14.25">
+      <c r="A153" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E153" t="s">
+        <v>74</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" ht="14.25">
+      <c r="A154" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="C154" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E154" t="s">
+        <v>69</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" ht="14.25">
+      <c r="A155" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C155" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="D155" s="6"/>
+      <c r="F155" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="156" ht="14.25">
+      <c r="A156" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="D156" s="6"/>
+      <c r="E156" t="s">
+        <v>69</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" ht="14.25">
+      <c r="A157" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="C157" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="D157" s="6"/>
+      <c r="F157" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="158" ht="14.25"/>
+    <row r="159" ht="14.25"/>
+    <row r="160" ht="14.25"/>
+    <row r="161" ht="14.25"/>
+    <row r="162" ht="14.25"/>
+    <row r="163" ht="14.25"/>
+    <row r="164" ht="14.25"/>
+    <row r="165" ht="14.25"/>
+    <row r="166" ht="14.25"/>
+    <row r="167" ht="14.25"/>
+    <row r="168" ht="14.25"/>
+    <row r="169" ht="14.25"/>
   </sheetData>
   <autoFilter ref="A1:F138"/>
-  <sortState ref="A2:F89" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="A2:A89"/>
+  <sortState ref="A2:F155" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A155"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -4260,87 +4730,87 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>334</v>
+      <c r="A1" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>337</v>
+      <c r="C2" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>340</v>
+      <c r="B3" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>343</v>
+      <c r="B4" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="5" ht="15">
       <c r="A5" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>347</v>
+        <v>380</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>351</v>
+      <c r="A6" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -4348,109 +4818,109 @@
         <v>265</v>
       </c>
       <c r="B7" t="s">
-        <v>352</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>353</v>
+        <v>388</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>389</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="B8" t="s">
-        <v>355</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>356</v>
+        <v>391</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>392</v>
       </c>
       <c r="D8" t="s">
-        <v>357</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>360</v>
-      </c>
-      <c r="D9" s="16"/>
+      <c r="A9" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>363</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>364</v>
+      <c r="A10" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>368</v>
+      <c r="A11" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>369</v>
+      <c r="C12" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>407</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>375</v>
+      <c r="D14" s="20" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add Groot database
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="446">
   <si>
     <t>database</t>
   </si>
@@ -1144,6 +1144,91 @@
     <t>Root.type</t>
   </si>
   <si>
+    <t>Groot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root_mycorrhizal colonization</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Specific_root_length</t>
+  </si>
+  <si>
+    <t>m/g</t>
+  </si>
+  <si>
+    <t>Root_N_concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root nitrogen concentration</t>
+  </si>
+  <si>
+    <t>mg/g</t>
+  </si>
+  <si>
+    <t>Mean_Root_diameter</t>
+  </si>
+  <si>
+    <t>Root_tissue_density</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="64"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>g/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="64"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>Lateral_spread</t>
+  </si>
+  <si>
+    <t>Root_Lateral_spread</t>
+  </si>
+  <si>
+    <t>cm/year</t>
+  </si>
+  <si>
+    <t>Root_mass_fraction</t>
+  </si>
+  <si>
+    <t>g/g</t>
+  </si>
+  <si>
+    <t>Root_C_concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root structural carbohydrate concentration</t>
+  </si>
+  <si>
+    <t>Rooting_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum rooting depth</t>
+  </si>
+  <si>
+    <t>Root_C_N_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root carbon-to-nitrogen ratio</t>
+  </si>
+  <si>
+    <t>mg/mg</t>
+  </si>
+  <si>
     <t>Database</t>
   </si>
   <si>
@@ -1183,6 +1268,56 @@
     <t xml:space="preserve">access via API</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="64"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Kühn, I., Durka, W., &amp; Klotz, S. (2004). BiolFlor: a new plant-trait database as a tool for plant invasion ecology. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color indexed="64"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Diversity and Distributions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="64"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color indexed="64"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="64"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">(5/6), 363-365.</t>
+    </r>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>Biolflor_41641.txt</t>
+  </si>
+  <si>
     <t>dcube</t>
   </si>
   <si>
@@ -1207,22 +1342,91 @@
     <t>Life_form_Dfevojan_2023.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Fitter, A. H. and Peat, H. J., 1994, The Ecological Flora Database, J. Ecol., 82, 415-425.</t>
+  </si>
+  <si>
+    <t>Ecoflora_41939.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theau J-P, Prud’homme F. 2021. FlorealData : Des traits de vie d’espèces végétales pour le calcul d’indices agronomiques et écologiques des communautés prairiales. Cah. Agric. 30: 36.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.15454/ADCQHT</t>
+  </si>
+  <si>
+    <t>FlorealData.xlsx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Weigelt, P., König, C. &amp; Kreft, H. (2020) GIFT - A Global Inventory of Floras and Traits for macroecology and biogeography. Journal of Biogeography, 47, 16-43. DOI: 10.1111/jbi.13623</t>
   </si>
   <si>
     <t>https://gift.uni-goettingen.de/home</t>
   </si>
   <si>
+    <t xml:space="preserve">Guerrero-Ramirez N, Mommer L, Freschet GT, Iversen CM, ... , Weigelt A. 2021. Global Root Traits (GRooT) Database. Global Ecology and Biogeography 30(1): 25-37</t>
+  </si>
+  <si>
+    <t>https://groot-database.github.io/GRooT/</t>
+  </si>
+  <si>
+    <t>GRooTAggregateSpeciesVersion.csv</t>
+  </si>
+  <si>
     <t>Hodgson_2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Hodgson, J., Jones, G., Charles, M., Stroud, E., Ater, M., Band, P., ... &amp; Bogaard, A. (2023). A functional trait database of arable weeds from Eurasia and North Africa.</t>
+    <t xml:space="preserve">Hodgson, J., Jones, G., Charles, M., Stroud, E., ... &amp; Bogaard, A. (2023). A functional trait database of arable weeds from Eurasia and North Africa.</t>
   </si>
   <si>
     <t>https://ora.ox.ac.uk/objects/uuid:abafafd9-e8a2-4e84-a339-0a11bf2858ae</t>
   </si>
   <si>
     <t>Functional+trait+database+of+arable+weeds+from+Eurasia+and+North+Africa.xlsx</t>
+  </si>
+  <si>
+    <t>Lososova_2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lososová Z., Axmanová I., Chytrý M., Midolo G., ... &amp; Thuiller W. (2023). Seed dispersal distance classes and dispersal modes for the European flora. Global Ecology and Biogeography.</t>
+  </si>
+  <si>
+    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/Lososova_et_al_2023_Dispersal_version2_2024-06-14.xlsx</t>
+  </si>
+  <si>
+    <t>Lososova_et_al_2023_Dispersal_version2_2024-06-14.xlsx</t>
+  </si>
+  <si>
+    <t>Midolo_2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midolo, G., Herben, T., Axmanová, I., Marcenò, C., ... &amp; Chytrý, M. (2023). Disturbance indicator values for European plants. Global Ecology and Biogeography, 32(1), 24-34.</t>
+  </si>
+  <si>
+    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/disturbance_indicator_values.xlsx</t>
+  </si>
+  <si>
+    <t>disturbance_indicator_values_Midolo_2023.xlsx</t>
+  </si>
+  <si>
+    <t>TraitSpVignes.xls</t>
+  </si>
+  <si>
+    <t>Tichy_2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tichý, L., Axmanová, I., Dengler, J., Guarino, R., Jansen, F., Midolo, G., ... &amp; Chytrý, M. (2023). Ellenberg‐type indicator values for European vascular plant species. Journal of Vegetation Science, 34(1), e13168.</t>
+  </si>
+  <si>
+    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/Indicator_values_Tichy_et_al%202022-11-29.xlsx</t>
+  </si>
+  <si>
+    <t>Ellenberg_Indicator_values_Tichy_2022.xlsx</t>
+  </si>
+  <si>
+    <t>Yvoz_ValPol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeurs polliniques estimees.csv</t>
   </si>
   <si>
     <t>LEDA</t>
@@ -1274,57 +1478,12 @@
   <si>
     <t>https://uol.de/en/landeco/research/leda</t>
   </si>
-  <si>
-    <t>Lososova_2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lososová Z., Axmanová I., Chytrý M., Midolo G., Abdulhak S., Karger D.N., Renaud J., Van Es J., Vittoz P. &amp; Thuiller W. (2023). Seed dispersal distance classes and dispersal modes for the European flora. Global Ecology and Biogeography.</t>
-  </si>
-  <si>
-    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/Lososova_et_al_2023_Dispersal_version2_2024-06-14.xlsx</t>
-  </si>
-  <si>
-    <t>Lososova_et_al_2023_Dispersal_version2_2024-06-14.xlsx</t>
-  </si>
-  <si>
-    <t>Midolo_2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midolo, G., Herben, T., Axmanová, I., Marcenò, C., Pätsch, R., Bruelheide, H., ... &amp; Chytrý, M. (2023). Disturbance indicator values for European plants. Global Ecology and Biogeography, 32(1), 24-34.</t>
-  </si>
-  <si>
-    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/disturbance_indicator_values.xlsx</t>
-  </si>
-  <si>
-    <t>disturbance_indicator_values_Midolo_2023.xlsx</t>
-  </si>
-  <si>
-    <t>TraitSpVignes.xls</t>
-  </si>
-  <si>
-    <t>Tichy_2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tichý, L., Axmanová, I., Dengler, J., Guarino, R., Jansen, F., Midolo, G., ... &amp; Chytrý, M. (2023). Ellenberg‐type indicator values for European vascular plant species. Journal of Vegetation Science, 34(1), e13168.</t>
-  </si>
-  <si>
-    <t>https://files.ibot.cas.cz/cevs/downloads/floraveg/Indicator_values_Tichy_et_al%202022-11-29.xlsx</t>
-  </si>
-  <si>
-    <t>Ellenberg_Indicator_values_Tichy_2022.xlsx</t>
-  </si>
-  <si>
-    <t>Yvoz_ValPol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valeurs polliniques estimees.csv</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13">
+  <fonts count="21">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -1358,20 +1517,34 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="10.500000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.000000"/>
+      <color indexed="64"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="12.000000"/>
       <color theme="1" tint="0"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="12.000000"/>
       <color theme="1" tint="0"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.000000"/>
+      <sz val="14.000000"/>
       <color theme="1" tint="0"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -1382,15 +1555,41 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="14.000000"/>
+      <color theme="1" tint="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <u/>
       <sz val="11.000000"/>
       <color theme="1" tint="0"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="14.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <u/>
       <sz val="11.000000"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1402,7 +1601,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -1455,11 +1654,26 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1481,9 +1695,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1499,21 +1710,58 @@
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="10" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="11" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="12" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="13" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="13" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="14" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="15" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="13" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="16" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="17" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="18" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="19" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="15" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="18" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="20" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="13" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="12" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="15" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2024,7 +2272,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A139" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A154" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2936,7 +3184,7 @@
       <c r="B57" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D57" s="2"/>
@@ -3044,7 +3292,7 @@
       <c r="D64" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="11" t="s">
         <v>133</v>
       </c>
       <c r="F64" s="6" t="s">
@@ -3064,7 +3312,7 @@
       <c r="D65" t="s">
         <v>136</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="11" t="s">
         <v>71</v>
       </c>
       <c r="F65" s="6" t="s">
@@ -3084,7 +3332,7 @@
       <c r="D66" t="s">
         <v>139</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="11" t="s">
         <v>71</v>
       </c>
       <c r="F66" s="6" t="s">
@@ -3104,7 +3352,7 @@
       <c r="D67" t="s">
         <v>142</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="11" t="s">
         <v>133</v>
       </c>
       <c r="F67" s="6" t="s">
@@ -3124,7 +3372,7 @@
       <c r="D68" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>133</v>
       </c>
       <c r="F68" s="6" t="s">
@@ -3144,7 +3392,7 @@
       <c r="D69" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F69" s="6" t="s">
@@ -3914,7 +4162,7 @@
       <c r="B111" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="6" t="s">
         <v>273</v>
       </c>
       <c r="E111" s="6" t="s">
@@ -3931,7 +4179,7 @@
       <c r="B112" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="6" t="s">
         <v>275</v>
       </c>
       <c r="E112" s="6" t="s">
@@ -3965,7 +4213,7 @@
       <c r="B114" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="6" t="s">
         <v>279</v>
       </c>
       <c r="E114" s="6" t="s">
@@ -3982,7 +4230,7 @@
       <c r="B115" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E115" s="6" t="s">
@@ -4410,7 +4658,7 @@
       <c r="C140" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="D140" s="13" t="s">
+      <c r="D140" s="12" t="s">
         <v>333</v>
       </c>
       <c r="F140" s="6" t="s">
@@ -4427,7 +4675,7 @@
       <c r="C141" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D141" s="14" t="s">
+      <c r="D141" s="13" t="s">
         <v>336</v>
       </c>
       <c r="F141" s="6" t="s">
@@ -4444,7 +4692,7 @@
       <c r="C142" t="s">
         <v>338</v>
       </c>
-      <c r="D142" s="15" t="s">
+      <c r="D142" s="14" t="s">
         <v>339</v>
       </c>
       <c r="F142" s="6" t="s">
@@ -4461,7 +4709,7 @@
       <c r="C143" t="s">
         <v>341</v>
       </c>
-      <c r="D143" s="15" t="s">
+      <c r="D143" s="14" t="s">
         <v>342</v>
       </c>
       <c r="E143" t="s">
@@ -4495,7 +4743,7 @@
       <c r="B145" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C145" s="6" t="s">
         <v>346</v>
       </c>
       <c r="E145" t="s">
@@ -4527,7 +4775,7 @@
       <c r="B147" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C147" s="6" t="s">
         <v>349</v>
       </c>
       <c r="D147" s="6"/>
@@ -4542,7 +4790,7 @@
       <c r="B148" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C148" s="6" t="s">
         <v>351</v>
       </c>
       <c r="D148" s="6"/>
@@ -4557,7 +4805,7 @@
       <c r="B149" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C149" s="6" t="s">
         <v>353</v>
       </c>
       <c r="D149" s="6"/>
@@ -4572,7 +4820,7 @@
       <c r="B150" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="C150" s="6" t="s">
         <v>355</v>
       </c>
       <c r="D150" s="6"/>
@@ -4587,7 +4835,7 @@
       <c r="B151" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="C151" s="6" t="s">
         <v>357</v>
       </c>
       <c r="D151" s="6"/>
@@ -4602,7 +4850,7 @@
       <c r="B152" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="C152" s="16" t="s">
+      <c r="C152" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="6"/>
@@ -4634,7 +4882,7 @@
       <c r="B154" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E154" t="s">
@@ -4651,7 +4899,7 @@
       <c r="B155" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="6" t="s">
         <v>362</v>
       </c>
       <c r="D155" s="6"/>
@@ -4666,7 +4914,7 @@
       <c r="B156" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="6" t="s">
         <v>364</v>
       </c>
       <c r="D156" s="6"/>
@@ -4684,7 +4932,7 @@
       <c r="B157" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="6" t="s">
         <v>366</v>
       </c>
       <c r="D157" s="6"/>
@@ -4692,16 +4940,188 @@
         <v>322</v>
       </c>
     </row>
-    <row r="158" ht="14.25"/>
-    <row r="159" ht="14.25"/>
-    <row r="160" ht="14.25"/>
-    <row r="161" ht="14.25"/>
-    <row r="162" ht="14.25"/>
-    <row r="163" ht="14.25"/>
-    <row r="164" ht="14.25"/>
-    <row r="165" ht="14.25"/>
-    <row r="166" ht="14.25"/>
-    <row r="167" ht="14.25"/>
+    <row r="158" ht="14.25">
+      <c r="A158" t="s">
+        <v>367</v>
+      </c>
+      <c r="B158" t="s">
+        <v>368</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="E158" t="s">
+        <v>369</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" ht="14.25">
+      <c r="A159" t="s">
+        <v>367</v>
+      </c>
+      <c r="B159" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="C159" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="E159" t="s">
+        <v>371</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" ht="14.25">
+      <c r="A160" t="s">
+        <v>367</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="E160" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="F160" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" ht="14.25">
+      <c r="A161" t="s">
+        <v>367</v>
+      </c>
+      <c r="B161" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="C161" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="E161" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F161" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" ht="14.25">
+      <c r="A162" t="s">
+        <v>367</v>
+      </c>
+      <c r="B162" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="C162" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="E162" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="163" ht="14.25">
+      <c r="A163" t="s">
+        <v>367</v>
+      </c>
+      <c r="B163" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C163" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="E163" t="s">
+        <v>380</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="164" ht="14.25">
+      <c r="A164" t="s">
+        <v>367</v>
+      </c>
+      <c r="B164" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C164" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="E164" t="s">
+        <v>382</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="165" ht="14.25">
+      <c r="A165" t="s">
+        <v>367</v>
+      </c>
+      <c r="B165" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="C165" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="D165" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="E165" t="s">
+        <v>374</v>
+      </c>
+      <c r="F165" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="166" ht="14.25">
+      <c r="A166" t="s">
+        <v>367</v>
+      </c>
+      <c r="B166" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C166" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="D166" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E166" t="s">
+        <v>69</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167" ht="14.25">
+      <c r="A167" t="s">
+        <v>367</v>
+      </c>
+      <c r="B167" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="C167" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D167" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="E167" t="s">
+        <v>389</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="168" ht="14.25"/>
     <row r="169" ht="14.25"/>
   </sheetData>
@@ -4725,219 +5145,281 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="13.7109375"/>
-    <col customWidth="1" min="2" max="2" width="41.57421875"/>
+    <col customWidth="1" min="1" max="1" width="18.00390625"/>
+    <col customWidth="1" min="2" max="2" width="80.421875"/>
+    <col customWidth="1" min="3" max="3" width="19.28125"/>
+    <col customWidth="1" min="4" max="4" width="71.7109375"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" ht="16.5">
+      <c r="A1" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" ht="18.75">
+      <c r="A2" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" ht="45.75" customHeight="1">
+      <c r="A4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="5" ht="33.75" customHeight="1">
+      <c r="A5" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" ht="48" customHeight="1">
+      <c r="A6" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" ht="32.25" customHeight="1">
+      <c r="A9" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" ht="33" customHeight="1">
+      <c r="A10" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" ht="28.5">
+      <c r="A11" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>368</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="19" t="s">
-        <v>371</v>
-      </c>
-      <c r="B2" s="20" t="s">
+      <c r="B11" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" ht="30.75" customHeight="1">
+      <c r="A12" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>425</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" ht="45.75" customHeight="1">
+      <c r="A13" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="14" ht="33.75" customHeight="1">
+      <c r="A14" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" ht="32.25" customHeight="1">
+      <c r="A15" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>385</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B7" t="s">
-        <v>388</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>389</v>
-      </c>
-      <c r="D7" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" t="s">
-        <v>390</v>
-      </c>
-      <c r="B8" t="s">
-        <v>391</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="D8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="20" t="s">
-        <v>394</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="C15" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="20" t="s">
-        <v>397</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>398</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>399</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>403</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="20" t="s">
+      <c r="D15" s="24" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" ht="48" customHeight="1">
+      <c r="A16" s="25" t="s">
+        <v>437</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>438</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>439</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75">
+      <c r="A17" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" s="20" t="s">
-        <v>406</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>407</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>408</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>411</v>
-      </c>
+      <c r="C17" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25"/>
+    <row r="19" ht="14.25"/>
+    <row r="24" ht="42.75">
+      <c r="A24" s="39" t="s">
+        <v>443</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>444</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="D24" s="39"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D14" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="A2:A14"/>
+  <sortState ref="A2:D17" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A17"/>
   </sortState>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C3"/>
     <hyperlink r:id="rId2" ref="C4"/>
-    <hyperlink r:id="rId3" ref="C5"/>
-    <hyperlink r:id="rId4" ref="C6"/>
-    <hyperlink r:id="rId5" ref="C7"/>
-    <hyperlink r:id="rId6" ref="C8"/>
-    <hyperlink r:id="rId7" ref="C9"/>
-    <hyperlink r:id="rId8" ref="C10"/>
-    <hyperlink r:id="rId9" ref="C11"/>
-    <hyperlink r:id="rId10" ref="C13"/>
+    <hyperlink r:id="rId3" ref="C6"/>
+    <hyperlink r:id="rId4" ref="C7"/>
+    <hyperlink r:id="rId5" ref="C9"/>
+    <hyperlink r:id="rId6" ref="C10"/>
+    <hyperlink r:id="rId7" ref="C11"/>
+    <hyperlink r:id="rId8" ref="C12"/>
+    <hyperlink r:id="rId9" ref="C13"/>
+    <hyperlink r:id="rId10" ref="C14"/>
+    <hyperlink r:id="rId11" ref="C16"/>
+    <hyperlink r:id="rId12" ref="C24"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
fix: harmonize metatrait.xslx and improve 05_explore_traits
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
   <si>
     <t>database</t>
   </si>
@@ -58,21 +58,33 @@
     <t xml:space="preserve">Refers to Grime’s CSR strategy model, which classifies plant species based on three primary ecological strategies:C (Competitor): Plants that thrive in stable environments with abundant resources.</t>
   </si>
   <si>
+    <t>Population</t>
+  </si>
+  <si>
     <t>categorical</t>
   </si>
   <si>
     <t>MaxLife</t>
   </si>
   <si>
-    <t>Max_Life</t>
+    <t>Plant.lifespan</t>
   </si>
   <si>
     <t xml:space="preserve">Refers to the maximum lifespan of the plant, generally expressed in years. It indicates whether a plant is:Annual, Biennial, Perennial</t>
   </si>
   <si>
+    <t xml:space="preserve">Whole plant</t>
+  </si>
+  <si>
     <t>GrassHerbLegTree</t>
   </si>
   <si>
+    <t>Growth.form</t>
+  </si>
+  <si>
+    <t>Morphology</t>
+  </si>
+  <si>
     <t xml:space="preserve">This is a growth form classification that identifies a plant’s general morphological type:Grass: Monocots in the Poaceae family; Herb: Non-woody dicot plants; Leg: Leguminous plants (often nitrogen-fixing); Tree: Woody plants with a single main stem.</t>
   </si>
   <si>
@@ -121,21 +133,30 @@
     <t>fruit</t>
   </si>
   <si>
+    <t>Fruit.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed dispersal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates the type of fruit produced by the plant. Examples include:Achene, Berry, Capsule, Drupe, Nut</t>
+  </si>
+  <si>
     <t>Fruit</t>
   </si>
   <si>
-    <t xml:space="preserve">Indicates the type of fruit produced by the plant. Examples include:Achene, Berry, Capsule, Drupe, Nut</t>
-  </si>
-  <si>
     <t>dissémination</t>
   </si>
   <si>
-    <t>Dissemination</t>
+    <t>Dispersal.mode</t>
   </si>
   <si>
     <t xml:space="preserve">Refers to the method of seed dispersal, such as:Anemochory: Wind; Zoochory: Animals,Hydrochory: Water; Autochory: Self-dispersal mechanisms (explosive, gravity).</t>
   </si>
   <si>
+    <t>Seed</t>
+  </si>
+  <si>
     <t>couleur_fleur</t>
   </si>
   <si>
@@ -148,6 +169,9 @@
     <t xml:space="preserve">Dominant color of the flower, which can play a role in attracting specific pollinators</t>
   </si>
   <si>
+    <t xml:space="preserve">Floral unit</t>
+  </si>
+  <si>
     <t>floraison</t>
   </si>
   <si>
@@ -166,16 +190,13 @@
     <t>FORMATION_VEGETALE</t>
   </si>
   <si>
-    <t>Plant.formation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refers to the growth structure or architectural form of the plant, e.g.:Rosette, Creeping, erect, tussock, climbing</t>
   </si>
   <si>
     <t>CARACTERISATION_ECOLOGIQUE_(HABITAT_OPTIMAL)</t>
   </si>
   <si>
-    <t>Optimal.habitat</t>
+    <t>Habitat</t>
   </si>
   <si>
     <t xml:space="preserve">Describes the preferred environmental conditions or ecological niche where the plant is most successful.</t>
@@ -190,13 +211,10 @@
     <t xml:space="preserve">Refers to the dominant or most common pigmentation of the plant's flower.</t>
   </si>
   <si>
-    <t xml:space="preserve">Floral unit</t>
-  </si>
-  <si>
     <t>leaf.area.mm2</t>
   </si>
   <si>
-    <t>Morphology</t>
+    <t>Leaf.area_mm2</t>
   </si>
   <si>
     <t xml:space="preserve">Leaf Area (in mm²) measures the surface area of a single leaf.</t>
@@ -214,6 +232,9 @@
     <t>leaf.area.per.leaf.dry.mass.m2.kg-1</t>
   </si>
   <si>
+    <t>SLA_m2.kg-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Specific Leaf Area (SLA), calculated as:Leaf Area (m²) / Leaf Dry Mass (kg)Expressed in m²/kg, it reflects the efficiency of resource use in leaves.</t>
   </si>
   <si>
@@ -223,6 +244,9 @@
     <t>leaf.carbon.content.per.leaf.nitrogen.content</t>
   </si>
   <si>
+    <t>Leaf.carbon.to.nitrogen.content_mg.g-1</t>
+  </si>
+  <si>
     <t>Chemistry</t>
   </si>
   <si>
@@ -235,6 +259,9 @@
     <t>leaf.dry.mass.g</t>
   </si>
   <si>
+    <t>Leaf.dry.mass_g</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leaf Dry Mass (in grams) refers to the mass of a fully dried individual leaf.</t>
   </si>
   <si>
@@ -244,13 +271,16 @@
     <t>leaf.dry.mass.per.leaf.fresh.mass.mg.g-1</t>
   </si>
   <si>
+    <t>Leaf.dry.mass.content_mg.g-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leaf dry mass content</t>
   </si>
   <si>
     <t>leaf.nitrogen.content.per.leaf.dry.mass.mg.g-1</t>
   </si>
   <si>
-    <t>chemistry</t>
+    <t>Leaf.nitrogen.content_mg.g-1</t>
   </si>
   <si>
     <t xml:space="preserve">Carbon Content (C) / Nitrogen Content (N)</t>
@@ -259,22 +289,19 @@
     <t>plant.flowering.begin.month</t>
   </si>
   <si>
-    <t xml:space="preserve">Flowering Phenology</t>
+    <t>Flowering_begin.month</t>
   </si>
   <si>
     <t xml:space="preserve">Month of onset of flowering</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>(1-12)</t>
   </si>
   <si>
     <t>seed.mass.mg</t>
   </si>
   <si>
-    <t xml:space="preserve">Seed Morphology</t>
+    <t>Seed.mass_mg</t>
   </si>
   <si>
     <t xml:space="preserve">Seed dry mass</t>
@@ -295,15 +322,15 @@
     <t>whole.plant.height.m</t>
   </si>
   <si>
+    <t>Plant.height_m</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plant size</t>
   </si>
   <si>
     <t xml:space="preserve">Plant height</t>
   </si>
   <si>
-    <t xml:space="preserve">Whole plant</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -313,31 +340,19 @@
     <t xml:space="preserve">Plant height (m)</t>
   </si>
   <si>
-    <t>Plant.height_m</t>
-  </si>
-  <si>
     <t xml:space="preserve">Seed mass (mg)</t>
   </si>
   <si>
-    <t>Seed.mass_mg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Efficient dispersal mode - common</t>
   </si>
   <si>
-    <t>Efficient.dispersal.mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seed dispersal</t>
-  </si>
-  <si>
     <t xml:space="preserve">The primary and most effective mechanism by which a plant’s seeds or propagules are dispersed away from the parent plant (anemochory, zoochory, barochory, autochry, anthropochory)</t>
   </si>
   <si>
     <t xml:space="preserve">Dispersal distance class (1-6)</t>
   </si>
   <si>
-    <t>Dispersal.distance.class</t>
+    <t>Dispersal.distance_class</t>
   </si>
   <si>
     <t xml:space="preserve">Typical distance that propagules (seeds or vegetative parts) travel from the parent plant, often grouped into classes such as: short distancev Short-distance: &lt;10 meters — typical of gravity or unassisted  dispersal. Medium-distance: 10–100 meters — often achieved by wind or small animalsLong-distance: &gt;100 meters — includes large birds, mammals, or water currents</t>
@@ -352,7 +367,7 @@
     <t xml:space="preserve">Plant Height</t>
   </si>
   <si>
-    <t>Plant_Height</t>
+    <t>Plant.height_cm</t>
   </si>
   <si>
     <t>cm</t>
@@ -391,7 +406,7 @@
     <t xml:space="preserve">Type biologique (Raunkier)</t>
   </si>
   <si>
-    <t>Type_Raunkier</t>
+    <t>Lifeform_Raunkier</t>
   </si>
   <si>
     <t xml:space="preserve">This refers to the Raunkiær life-form classification system, which categorizes plants based on the position of their perennating (survival) organs during unfavorable seasons (phanerphyte; therophyte etc)</t>
@@ -475,7 +490,7 @@
     <t>quantite_nectar</t>
   </si>
   <si>
-    <t>quantite.nectar</t>
+    <t>Nectar.quantity</t>
   </si>
   <si>
     <t xml:space="preserve">Flower ressources</t>
@@ -487,10 +502,10 @@
     <t>quantite_pollen</t>
   </si>
   <si>
-    <t>quantite.pollen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">his trait measures the amount of pollen produced by a flower or pla</t>
+    <t>Pollen.quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This trait measures the amount of pollen produced by a flower</t>
   </si>
   <si>
     <t>Couleur</t>
@@ -502,7 +517,7 @@
     <t>UV_reflection_periphery</t>
   </si>
   <si>
-    <t>UV.reflection.periphery</t>
+    <t>Flower.UV.reflectanceperiphery</t>
   </si>
   <si>
     <t xml:space="preserve">Refers to the ability of the outer parts of the flower (petals/lobes) to reflect ultraviolet (UV) light. T</t>
@@ -511,7 +526,7 @@
     <t>UV_reflection_centre</t>
   </si>
   <si>
-    <t>UV.reflection.centre</t>
+    <t>Flower.UV.reflectance.centre</t>
   </si>
   <si>
     <t xml:space="preserve">Measures the UV reflectance of the central region of the flower (often around the reproductive organs)</t>
@@ -520,6 +535,9 @@
     <t>Symetrie</t>
   </si>
   <si>
+    <t>Floral.symmetry</t>
+  </si>
+  <si>
     <t xml:space="preserve">Describes the floral symmetry: radial, bilateral, assymetric</t>
   </si>
   <si>
@@ -586,9 +604,6 @@
     <t>fruit_type</t>
   </si>
   <si>
-    <t>fruit.type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description of the ecological characteristics of the fruit that are related to seed dispersal</t>
   </si>
   <si>
@@ -598,7 +613,7 @@
     <t>dia_type</t>
   </si>
   <si>
-    <t>dia.type</t>
+    <t>Diaspore.type</t>
   </si>
   <si>
     <t xml:space="preserve">Description of the morphological structure that acts as the diaspore, i.e. the diasporsal unit</t>
@@ -610,7 +625,7 @@
     <t>dia_exposure</t>
   </si>
   <si>
-    <t>dia.exposure</t>
+    <t>Diaspore.exposure</t>
   </si>
   <si>
     <t xml:space="preserve">Diaspore exposure, accessibility of dispersal vectors to the diaspores within the infructescence;</t>
@@ -622,7 +637,7 @@
     <t>dia_mass</t>
   </si>
   <si>
-    <t>dia.mass.mg</t>
+    <t>Diaspore.mass_mg</t>
   </si>
   <si>
     <t xml:space="preserve">Seed morphology</t>
@@ -634,7 +649,7 @@
     <t>dia_height</t>
   </si>
   <si>
-    <t>dia.height.mm</t>
+    <t>Diaspore.height_mm</t>
   </si>
   <si>
     <t xml:space="preserve">diaspore height, i.e. the shortest axis perpendicular to length and width, including all appendages</t>
@@ -646,7 +661,7 @@
     <t>rank_ane</t>
   </si>
   <si>
-    <t>rank.ane</t>
+    <t>Anemochory_rank</t>
   </si>
   <si>
     <t xml:space="preserve">anemochory ranking index, assess how well a species is adapted to anemochory (wind dispersal)</t>
@@ -658,7 +673,7 @@
     <t>rank_hydro</t>
   </si>
   <si>
-    <t>rank.hydro</t>
+    <t>Hydrochory_rank</t>
   </si>
   <si>
     <t xml:space="preserve">hydrochory ranking index, assess how well a species is adapted to hydrochory (water dispersal)</t>
@@ -667,7 +682,7 @@
     <t>rank_epi_wool</t>
   </si>
   <si>
-    <t>rank.epi.wool</t>
+    <t>Epizoochory_rank</t>
   </si>
   <si>
     <t xml:space="preserve">epizoochory ranking index, assess how well a species is adapted to epizoochory (external animal dispersal)</t>
@@ -682,9 +697,6 @@
     <t>SLA.mm2.mg-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Leaf Morphology</t>
-  </si>
-  <si>
     <t xml:space="preserve">Specific leaf area</t>
   </si>
   <si>
@@ -694,7 +706,7 @@
     <t>LOGCANH</t>
   </si>
   <si>
-    <t>Log2.canopy.height</t>
+    <t>Canopy.height_log2</t>
   </si>
   <si>
     <t xml:space="preserve">Canopy height (converted to log2 bins)</t>
@@ -706,7 +718,7 @@
     <t>LOGCAND</t>
   </si>
   <si>
-    <t>Log2.canopy.diameter</t>
+    <t>Canopy.diameter_log2</t>
   </si>
   <si>
     <t xml:space="preserve">Canopy diameter (converted to log2 bins)</t>
@@ -715,13 +727,13 @@
     <t>VEGPROP</t>
   </si>
   <si>
-    <t>Vegprop</t>
+    <t>Vegetative.propagation</t>
   </si>
   <si>
     <t xml:space="preserve">Plant morphology</t>
   </si>
   <si>
-    <t xml:space="preserve">Vegetative propagation  of perennials</t>
+    <t xml:space="preserve">Vegetative propagation of perennials</t>
   </si>
   <si>
     <t>(0,1)</t>
@@ -733,7 +745,7 @@
     <t>LIFEHIST</t>
   </si>
   <si>
-    <t>Lifehist</t>
+    <t>Lifecycle</t>
   </si>
   <si>
     <t xml:space="preserve">Life history</t>
@@ -748,6 +760,9 @@
     <t>Growth_form_1</t>
   </si>
   <si>
+    <t>Growth.form_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">herb, shrub, tree, other</t>
   </si>
   <si>
@@ -760,43 +775,49 @@
     <t>Growth_form_2</t>
   </si>
   <si>
+    <t>Growth.form_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">herb, graminoid, forb, subshrub, shrub, tree, palm, other</t>
   </si>
   <si>
     <t>Plant_height_max</t>
   </si>
   <si>
-    <t>Plant_height_max_m</t>
+    <t>Plant.height_max_m</t>
   </si>
   <si>
     <t>Plant_height_min</t>
   </si>
   <si>
-    <t>Plant_height_min_m</t>
+    <t>Plant.height_min_m</t>
   </si>
   <si>
     <t>Photosynthetic_pathway</t>
   </si>
   <si>
+    <t>Photosynthetic.pathway</t>
+  </si>
+  <si>
     <t xml:space="preserve">C3, C4, CAM</t>
   </si>
   <si>
     <t>Seed_mass_mean</t>
   </si>
   <si>
-    <t>Seed_mass_mean_g</t>
+    <t>Seed.mass_g</t>
   </si>
   <si>
     <t>Plant_height_mean</t>
   </si>
   <si>
-    <t>Plant_height_mean_m</t>
+    <t>Plant.height_mean_m</t>
   </si>
   <si>
     <t>Leaf_length_mean</t>
   </si>
   <si>
-    <t>Leaf_length_mean_cm</t>
+    <t>Leaf.length_cm</t>
   </si>
   <si>
     <t xml:space="preserve">Leaf length</t>
@@ -805,13 +826,16 @@
     <t>Dispersal_syndrome_1</t>
   </si>
   <si>
+    <t>Dispersal.mode_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">anemochorous, zoochorous, autochorous, hydrochorous, unspecialized</t>
   </si>
   <si>
     <t>Leaf_width_mean</t>
   </si>
   <si>
-    <t>Leaf_width_mean_cm</t>
+    <t>Leaf.width_cm</t>
   </si>
   <si>
     <t xml:space="preserve">Leaf width</t>
@@ -820,37 +844,52 @@
     <t>Dispersal_syndrome_2</t>
   </si>
   <si>
+    <t>Dispersal.mode_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">anemochorous, anthropochorous, autochorous, endozoochorous, epizoochorous, hydrochorous, myrmecochorous, unspecialized, zoochorous</t>
   </si>
   <si>
     <t>Pollination_syndrome_1</t>
   </si>
   <si>
+    <t>Pollination.syndrome_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">biotic, abiotic</t>
   </si>
   <si>
     <t>Pollination_syndrome_2</t>
   </si>
   <si>
+    <t>Pollination.syndrome_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">wind, water, insect, bird, bat, other</t>
   </si>
   <si>
     <t>Pollination_syndrome_3</t>
   </si>
   <si>
+    <t>Pollination.syndrome_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">wind, water, bee, beetle, ant, butterfly, moth, fly, insect, bird, bat, other</t>
   </si>
   <si>
     <t>Fruit_colour</t>
   </si>
   <si>
+    <t>Fruit.colour</t>
+  </si>
+  <si>
     <t xml:space="preserve">red, pink, blue, yellow, orange, green, white, violet, black, grey, brown, other</t>
   </si>
   <si>
     <t>Flower_length_max</t>
   </si>
   <si>
-    <t>Flower_length_max_cm</t>
+    <t>Flower.length_max_cm</t>
   </si>
   <si>
     <t xml:space="preserve">calculate floral area with length and width?</t>
@@ -862,13 +901,16 @@
     <t>Flower_length_min</t>
   </si>
   <si>
-    <t>Flower_length_min_cm</t>
+    <t>Flower.length_min_cm</t>
   </si>
   <si>
     <t>Leaf_size_mean</t>
   </si>
   <si>
-    <t>Leaf_size_mean_cm2</t>
+    <t>Leaf.area_cm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf area measures the surface area of a single leaf.</t>
   </si>
   <si>
     <t>cm²</t>
@@ -883,19 +925,19 @@
     <t>Flower_width_max</t>
   </si>
   <si>
-    <t>Flower_width_max_cm</t>
+    <t>Flower.width_max_cm</t>
   </si>
   <si>
     <t>Flower_width_min</t>
   </si>
   <si>
-    <t>Flower_width_min_cm</t>
+    <t>Flower.width_min_cm</t>
   </si>
   <si>
     <t>SLA_mean</t>
   </si>
   <si>
-    <t>SLA_mean_cm2.g-1</t>
+    <t>SLA_cm2.g-1</t>
   </si>
   <si>
     <t xml:space="preserve">Specific leaf area (leaf area divided by leaf dry mass)</t>
@@ -910,16 +952,13 @@
     <t>Coul</t>
   </si>
   <si>
-    <t>Flower_color</t>
-  </si>
-  <si>
     <t xml:space="preserve">Couleur dominante de la ﬂeur</t>
   </si>
   <si>
     <t>SSI</t>
   </si>
   <si>
-    <t>Specialization_index</t>
+    <t>Grassland.specialization</t>
   </si>
   <si>
     <t xml:space="preserve">Grassland Community Specialization Index</t>
@@ -937,9 +976,6 @@
     <t>TailMoy</t>
   </si>
   <si>
-    <t>Plant_Height_cm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Taille des espèces non graminéennes</t>
   </si>
   <si>
@@ -976,15 +1012,12 @@
     <t xml:space="preserve">Flower UV light reflectance</t>
   </si>
   <si>
-    <t>Flower.UV.light.reflectance</t>
+    <t>Flower.UV.reflectance</t>
   </si>
   <si>
     <t xml:space="preserve">Plant lifespan (longevity)</t>
   </si>
   <si>
-    <t>Plant.lifespan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Species strategy type according to Grime</t>
   </si>
   <si>
@@ -997,15 +1030,15 @@
     <t xml:space="preserve">Plant reproductive phenology timing (flowering time)</t>
   </si>
   <si>
-    <t>Plant.flowering</t>
-  </si>
-  <si>
     <t xml:space="preserve">Root rooting depth</t>
   </si>
   <si>
     <t>Root.depth_m</t>
   </si>
   <si>
+    <t>Root</t>
+  </si>
+  <si>
     <t xml:space="preserve">Root type, root architecture</t>
   </si>
   <si>
@@ -1018,18 +1051,27 @@
     <t xml:space="preserve">Root_mycorrhizal colonization</t>
   </si>
   <si>
+    <t>Root.mycorrhizal.colonization</t>
+  </si>
+  <si>
     <t>%</t>
   </si>
   <si>
     <t>Specific_root_length</t>
   </si>
   <si>
+    <t>Specific.root.length_m.g-1</t>
+  </si>
+  <si>
     <t>m/g</t>
   </si>
   <si>
     <t>Root_N_concentration</t>
   </si>
   <si>
+    <t>Root.N.concentration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Root nitrogen concentration</t>
   </si>
   <si>
@@ -1039,16 +1081,22 @@
     <t>Mean_Root_diameter</t>
   </si>
   <si>
+    <t>Root.diameter_mm</t>
+  </si>
+  <si>
     <t>Root_tissue_density</t>
   </si>
   <si>
+    <t>Root.tissue.density_g.cm-3</t>
+  </si>
+  <si>
     <t>g/cm3</t>
   </si>
   <si>
     <t>Lateral_spread</t>
   </si>
   <si>
-    <t>Root_Lateral_spread</t>
+    <t>Root.lateral.spread_cm.yr-1</t>
   </si>
   <si>
     <t>cm/year</t>
@@ -1057,12 +1105,18 @@
     <t>Root_mass_fraction</t>
   </si>
   <si>
+    <t>Root.mass.fraction</t>
+  </si>
+  <si>
     <t>g/g</t>
   </si>
   <si>
     <t>Root_C_concentration</t>
   </si>
   <si>
+    <t>Root.C.concentration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Root structural carbohydrate concentration</t>
   </si>
   <si>
@@ -1073,6 +1127,9 @@
   </si>
   <si>
     <t>Root_C_N_ratio</t>
+  </si>
+  <si>
+    <t>Root.C.N.ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Root carbon-to-nitrogen ratio</t>
@@ -1270,10 +1327,17 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1794,7 +1858,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D106" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1803,7 +1867,8 @@
     <col bestFit="1" min="1" max="1" width="12.7109375"/>
     <col bestFit="1" min="2" max="2" width="48.48046875"/>
     <col bestFit="1" min="3" max="3" width="41.171875"/>
-    <col bestFit="1" min="4" max="4" width="18.54296875"/>
+    <col customWidth="1" min="4" max="4" width="11.7109375"/>
+    <col customWidth="1" min="5" max="5" width="57.7109375"/>
     <col bestFit="1" min="6" max="6" width="11.57421875"/>
     <col customWidth="1" min="7" max="7" width="16.28125"/>
   </cols>
@@ -1850,8 +1915,11 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -1859,19 +1927,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -1879,708 +1950,745 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
+        <v>62</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
       <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
         <v>78</v>
       </c>
-      <c r="F21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
-      </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" t="s">
-        <v>82</v>
+        <v>91</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>85</v>
+        <v>94</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" t="s">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" t="s">
         <v>96</v>
       </c>
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" t="s">
-        <v>87</v>
-      </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H27" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F31" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
@@ -2589,1718 +2697,1871 @@
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="G36" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H36" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H37" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G38" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G39" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H39" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G40" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="H40" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G41" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="H41" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="H43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
-      </c>
-      <c r="C44" t="s">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E44" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="G45" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H45" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D46" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E46" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G46" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H46" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D47" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E48" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B49" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G50" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H50" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="E51" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G51" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" t="s">
         <v>182</v>
       </c>
-      <c r="D52" t="s">
-        <v>176</v>
-      </c>
       <c r="E52" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="G52" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H52" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C53" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="E53" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="G53" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H53" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C54" t="s">
-        <v>189</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>190</v>
+        <v>195</v>
+      </c>
+      <c r="F54" t="s">
+        <v>41</v>
       </c>
       <c r="G54" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="H54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C55" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G55" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="H55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B56" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C56" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E56" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="G56" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="H56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C57" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D57" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E57" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="G57" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H57" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D58" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E58" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G58" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H58" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C59" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E59" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="G59" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="H59" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C60" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D60" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E60" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G60" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="H60" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B61" t="s">
-        <v>215</v>
-      </c>
-      <c r="C61" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D61" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" t="s">
+        <v>222</v>
+      </c>
+      <c r="G61" t="s">
         <v>216</v>
       </c>
-      <c r="D61" t="s">
-        <v>103</v>
-      </c>
-      <c r="E61" t="s">
-        <v>217</v>
-      </c>
-      <c r="G61" t="s">
-        <v>211</v>
-      </c>
       <c r="H61" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B62" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C62" t="s">
-        <v>220</v>
-      </c>
-      <c r="D62" t="s">
-        <v>221</v>
+        <v>225</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E62" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G62" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="H62" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B63" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C63" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D63" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E63" t="s">
-        <v>226</v>
+        <v>230</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G63" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H63" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C64" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D64" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>230</v>
+        <v>234</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G64" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H64" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D65" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E65" t="s">
-        <v>234</v>
+        <v>238</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G65" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H65" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
-      </c>
-      <c r="C66" t="s">
-        <v>238</v>
+        <v>241</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
       </c>
       <c r="E66" t="s">
-        <v>239</v>
+        <v>243</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="G66" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B67" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
-        <v>242</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
+        <v>247</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G67" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B68" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C68" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
       </c>
+      <c r="F68" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="G68" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B69" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C69" t="s">
-        <v>246</v>
-      </c>
-      <c r="D69" t="s">
-        <v>11</v>
+        <v>252</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G69" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="H69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B70" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C70" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F70" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G70" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H70" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B71" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C71" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D71" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F71" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G71" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H71" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C72" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="H72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>254</v>
-      </c>
-      <c r="C73" t="s">
-        <v>255</v>
-      </c>
-      <c r="D73" t="s">
-        <v>85</v>
-      </c>
-      <c r="E73" t="s">
-        <v>86</v>
-      </c>
-      <c r="F73" t="s">
-        <v>87</v>
+        <v>261</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G73" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="H73" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B74" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C74" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D74" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E74" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F74" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G74" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H74" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="C75" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E75" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="F75" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G75" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H75" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B76" t="s">
-        <v>261</v>
-      </c>
-      <c r="C76" t="s">
-        <v>261</v>
+        <v>268</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="D76" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="G76" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B77" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C77" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D77" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E77" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="F77" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G77" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H77" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>266</v>
-      </c>
-      <c r="C78" t="s">
-        <v>266</v>
+        <v>274</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="G78" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="H78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="C79" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D79" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G79" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="H79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C80" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D80" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G80" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="H80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="C81" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="D81" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G81" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="H81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B82" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="C82" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="D82" t="s">
-        <v>202</v>
+        <v>207</v>
+      </c>
+      <c r="F82" t="s">
+        <v>41</v>
       </c>
       <c r="G82" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="H82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="C83" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="D83" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E83" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="F83" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H83" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B84" t="s">
-        <v>279</v>
-      </c>
-      <c r="C84" t="s">
-        <v>279</v>
-      </c>
-      <c r="D84" t="s">
-        <v>41</v>
+        <v>292</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E84" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F84" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G84" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="H84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="D85" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E85" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="F85" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G85" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H85" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="C86" t="s">
-        <v>283</v>
-      </c>
-      <c r="D86" t="s">
-        <v>59</v>
+        <v>296</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G86" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="H86" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D87" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G87" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="H87" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B88" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C88" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D88" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E88" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="F88" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G88" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H88" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B89" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="C89" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="D89" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E89" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="F89" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G89" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H89" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C90" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="D90" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E90" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="F90" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G90" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="H90" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B91" t="s">
-        <v>296</v>
-      </c>
-      <c r="C91" t="s">
-        <v>297</v>
+        <v>310</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E91" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="H91" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B92" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C92" t="s">
-        <v>300</v>
+        <v>313</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E92" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="H92" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B93" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="C93" t="s">
-        <v>303</v>
+        <v>316</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E93" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="H93" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B94" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="C94" t="s">
-        <v>306</v>
+        <v>116</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>307</v>
+        <v>319</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G94" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H94" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G95" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H95" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B96" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="C96" t="s">
-        <v>310</v>
+        <v>322</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G96" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H96" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B97" t="s">
-        <v>311</v>
-      </c>
-      <c r="C97" t="s">
-        <v>40</v>
+        <v>323</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="H97" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B98" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="C98" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="H98" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B99" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C99" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="H99" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B100" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C100" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="H100" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B101" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C101" t="s">
-        <v>319</v>
+        <v>331</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="H101" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B102" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C102" t="s">
-        <v>321</v>
+        <v>16</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H102" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B103" t="s">
-        <v>322</v>
-      </c>
-      <c r="C103" t="s">
+        <v>333</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H103" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B104" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C104" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G104" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H104" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B105" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="C105" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G105" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H105" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B106" t="s">
-        <v>325</v>
-      </c>
-      <c r="C106" t="s">
-        <v>326</v>
+        <v>336</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H106" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B107" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C107" t="s">
-        <v>328</v>
+        <v>338</v>
+      </c>
+      <c r="F107" t="s">
+        <v>339</v>
       </c>
       <c r="G107" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H107" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B108" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="C108" t="s">
-        <v>330</v>
+        <v>341</v>
+      </c>
+      <c r="F108" t="s">
+        <v>339</v>
       </c>
       <c r="H108" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B109" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C109" t="s">
-        <v>332</v>
+        <v>344</v>
+      </c>
+      <c r="F109" t="s">
+        <v>339</v>
       </c>
       <c r="G109" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="H109" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B110" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="C110" t="s">
-        <v>334</v>
+        <v>347</v>
+      </c>
+      <c r="F110" t="s">
+        <v>339</v>
       </c>
       <c r="G110" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="H110" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B111" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C111" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E111" t="s">
-        <v>337</v>
+        <v>351</v>
+      </c>
+      <c r="F111" t="s">
+        <v>339</v>
       </c>
       <c r="G111" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="H111" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B112" t="s">
+        <v>353</v>
+      </c>
+      <c r="C112" t="s">
+        <v>354</v>
+      </c>
+      <c r="F112" t="s">
         <v>339</v>
       </c>
-      <c r="C112" t="s">
-        <v>339</v>
-      </c>
       <c r="G112" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H112" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B113" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="C113" t="s">
-        <v>340</v>
+        <v>356</v>
+      </c>
+      <c r="F113" t="s">
+        <v>339</v>
       </c>
       <c r="G113" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
       <c r="H113" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B114" t="s">
-        <v>342</v>
+        <v>358</v>
       </c>
       <c r="C114" t="s">
-        <v>343</v>
+        <v>359</v>
+      </c>
+      <c r="F114" t="s">
+        <v>339</v>
       </c>
       <c r="G114" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="H114" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B115" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="C115" t="s">
-        <v>345</v>
+        <v>362</v>
+      </c>
+      <c r="F115" t="s">
+        <v>339</v>
       </c>
       <c r="G115" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
       <c r="H115" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B116" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="C116" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
       <c r="E116" t="s">
-        <v>348</v>
+        <v>366</v>
+      </c>
+      <c r="F116" t="s">
+        <v>339</v>
       </c>
       <c r="G116" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="H116" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B117" t="s">
-        <v>349</v>
-      </c>
-      <c r="C117" t="s">
-        <v>349</v>
+        <v>367</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="E117" t="s">
-        <v>350</v>
+        <v>368</v>
+      </c>
+      <c r="F117" t="s">
+        <v>339</v>
       </c>
       <c r="G117" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="H117" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B118" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="C118" t="s">
-        <v>351</v>
+        <v>370</v>
       </c>
       <c r="E118" t="s">
-        <v>352</v>
+        <v>371</v>
+      </c>
+      <c r="F118" t="s">
+        <v>339</v>
       </c>
       <c r="G118" t="s">
-        <v>353</v>
+        <v>372</v>
       </c>
       <c r="H118" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4318,7 +4579,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.8515625"/>
     <col customWidth="1" min="2" max="2" width="82.7109375"/>
@@ -4326,213 +4587,213 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>355</v>
+      <c r="A1" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>374</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>357</v>
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
+      <c r="A2" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="D2" t="s">
-        <v>360</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" ht="28.5">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>361</v>
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>380</v>
       </c>
       <c r="C3" t="s">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="D3" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" ht="42.75">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>364</v>
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="C4" t="s">
-        <v>365</v>
+        <v>384</v>
       </c>
       <c r="D4" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" ht="28.5">
-      <c r="A5" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>367</v>
+      <c r="A5" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>386</v>
       </c>
       <c r="C5" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="D5" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" ht="42.75">
-      <c r="A6" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>371</v>
+      <c r="A6" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>390</v>
       </c>
       <c r="C6" t="s">
-        <v>372</v>
+        <v>391</v>
       </c>
       <c r="D6" t="s">
-        <v>373</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>374</v>
+      <c r="A7" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>393</v>
       </c>
       <c r="C7" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="D7" t="s">
-        <v>375</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" ht="28.5">
-      <c r="A8" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>376</v>
+      <c r="A8" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>395</v>
       </c>
       <c r="C8" t="s">
-        <v>377</v>
+        <v>396</v>
       </c>
       <c r="D8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" ht="28.5">
+      <c r="A9" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="C9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="10" ht="28.5">
+      <c r="A10" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="C10" t="s">
+        <v>401</v>
+      </c>
+      <c r="D10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" ht="28.5">
+      <c r="A11" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" t="s">
+        <v>405</v>
+      </c>
+      <c r="D11" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" ht="28.5">
+      <c r="A12" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C12" t="s">
+        <v>409</v>
+      </c>
+      <c r="D12" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="9" ht="28.5">
-      <c r="A9" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="C9" t="s">
-        <v>380</v>
-      </c>
-      <c r="D9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" ht="28.5">
-      <c r="A10" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="C10" t="s">
-        <v>382</v>
-      </c>
-      <c r="D10" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="11" ht="28.5">
-      <c r="A11" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" t="s">
-        <v>386</v>
-      </c>
-      <c r="D11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" ht="28.5">
-      <c r="A12" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="C12" t="s">
-        <v>390</v>
-      </c>
-      <c r="D12" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>359</v>
-      </c>
       <c r="D13" t="s">
-        <v>392</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" ht="42.75">
-      <c r="A14" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>394</v>
+      <c r="A14" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>413</v>
       </c>
       <c r="C14" t="s">
-        <v>395</v>
+        <v>414</v>
       </c>
       <c r="D14" t="s">
-        <v>396</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>47</v>
+      <c r="A15" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>359</v>
+        <v>378</v>
       </c>
       <c r="D15" t="s">
-        <v>398</v>
+        <v>417</v>
       </c>
     </row>
     <row r="16"/>

</xml_diff>

<commit_message>
feat: update species list with ANN files from Guillaume and add CLO-PLA trait database
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="469">
   <si>
     <t>database</t>
   </si>
@@ -1138,6 +1138,146 @@
     <t>mg/mg</t>
   </si>
   <si>
+    <t>Root_dry_matter_content</t>
+  </si>
+  <si>
+    <t>Root.dry.matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root dry mass divided by root fresh mass</t>
+  </si>
+  <si>
+    <t>Root_length_density_volume</t>
+  </si>
+  <si>
+    <t>Root.length.density_cm.cm-3</t>
+  </si>
+  <si>
+    <t>cm/cm3</t>
+  </si>
+  <si>
+    <t>CLO-PLA</t>
+  </si>
+  <si>
+    <t>offspring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of offspring shoots per parent shoot.</t>
+  </si>
+  <si>
+    <t>offspring_wsmall</t>
+  </si>
+  <si>
+    <t>offspring.wsmall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of offspring per parent shoot including offspring of small size. Small offspring are defined as clonal offspring for which it took more years to attain a size comparable with other clonal offspring of the plant; they usually resemble seedlings.</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>lateral.spread_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lateral spread per year</t>
+  </si>
+  <si>
+    <t>clonalindex</t>
+  </si>
+  <si>
+    <t>clonal.index</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>FR_GRAS_FLOR</t>
+  </si>
+  <si>
+    <t>corola_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floral accessibility</t>
+  </si>
+  <si>
+    <t>corola_w</t>
+  </si>
+  <si>
+    <t>floral_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floral morphology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of the largest visible surface of the FU, considered to have a rectangular or circular shape depending of the species</t>
+  </si>
+  <si>
+    <t>mm²</t>
+  </si>
+  <si>
+    <t>Floral_unit_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of the floral unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower stamen / filament position relative to flower surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The distance between the filament and the constricting part of the flower, i.e. positive values = filament above the floral surface and negative filament = stylus hidden in nectar tubes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower stamen length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum length of the filament</t>
+  </si>
+  <si>
+    <t>flower_by_UF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of open flowers per FU</t>
+  </si>
+  <si>
+    <t>flower_height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortest distance between the top FU of an individual and the ground</t>
+  </si>
+  <si>
+    <t>nectar_sugar_content</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of sugar in nectar produced per flower after
+24 h of bagging, calculated from measurements of
+nectar volume and sugar concentration</t>
+  </si>
+  <si>
+    <t>Flower</t>
+  </si>
+  <si>
+    <t>µg.flower-1.day-1</t>
+  </si>
+  <si>
+    <t>nectar_tube_depth</t>
+  </si>
+  <si>
+    <t>nectar_veg_scale</t>
+  </si>
+  <si>
+    <t>pollen_grain_volume</t>
+  </si>
+  <si>
+    <t>pollen_quantity</t>
+  </si>
+  <si>
+    <t>pollen_volume</t>
+  </si>
+  <si>
     <t>Database</t>
   </si>
   <si>
@@ -1186,6 +1326,15 @@
     <t>Biolflor_41641.txt</t>
   </si>
   <si>
+    <t xml:space="preserve">Klimešová, J., Danihelka, J., Chrtek, J., de Bello, F., &amp; Herben, T. (2017). CLO‐PLA: a database of clonal and bud‐bank traits of the Central European flora.</t>
+  </si>
+  <si>
+    <t>https://esajournals.onlinelibrary.wiley.com/action/downloadSupplement?doi=10.1002%2Fecy.1745&amp;file=ecy1745-sup-0001-DataS1.zip</t>
+  </si>
+  <si>
+    <t>CLO-PLA-traits.txt</t>
+  </si>
+  <si>
     <t>Dcube</t>
   </si>
   <si>
@@ -1211,6 +1360,12 @@
   </si>
   <si>
     <t>FlorealData.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base traits floraux compilée par Alban Langlois</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t xml:space="preserve">Weigelt, P., König, C. &amp; Kreft, H. (2020) GIFT - A Global Inventory of Floras and Traits for macroecology and biogeography. Journal of Biogeography, 47, 16-43. DOI: 10.1111/jbi.13623</t>
@@ -1277,7 +1432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -1290,6 +1445,30 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1327,7 +1506,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1336,18 +1515,46 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1858,13 +2065,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A104" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="12.7109375"/>
+    <col customWidth="1" min="1" max="1" width="20.421875"/>
     <col bestFit="1" min="2" max="2" width="48.48046875"/>
     <col bestFit="1" min="3" max="3" width="41.171875"/>
     <col customWidth="1" min="4" max="4" width="11.7109375"/>
@@ -3409,7 +3616,7 @@
       <c r="E66" t="s">
         <v>243</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G66" t="s">
@@ -3878,7 +4085,7 @@
       <c r="D86" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="2" t="s">
         <v>297</v>
       </c>
       <c r="F86" s="2" t="s">
@@ -4563,6 +4770,392 @@
       <c r="H118" t="s">
         <v>69</v>
       </c>
+    </row>
+    <row r="119" ht="14.25">
+      <c r="A119" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" ht="14.25">
+      <c r="A120" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" ht="14.25">
+      <c r="A121" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C121" t="s">
+        <v>380</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" ht="14.25">
+      <c r="A122" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" ht="14.25">
+      <c r="A123" t="s">
+        <v>379</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="124" ht="14.25">
+      <c r="A124" t="s">
+        <v>379</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H124" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" ht="14.25">
+      <c r="A125" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="4"/>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="A126" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="C126" s="2"/>
+      <c r="D126" t="s">
+        <v>393</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="4"/>
+    </row>
+    <row r="127" ht="14.25">
+      <c r="A127" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E127" t="s">
+        <v>397</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="H127" s="4"/>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="A128" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E128" t="s">
+        <v>400</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H128" s="4"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="A129" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="4"/>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E130" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="4"/>
+    </row>
+    <row r="131" ht="14.25">
+      <c r="A131" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="4"/>
+    </row>
+    <row r="132" ht="14.25">
+      <c r="A132" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E132" t="s">
+        <v>408</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G132" s="2"/>
+      <c r="H132" s="4"/>
+    </row>
+    <row r="133" ht="14.25">
+      <c r="A133" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E133" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="G133" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="H133" s="4"/>
+    </row>
+    <row r="134" ht="14.25">
+      <c r="A134" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="4"/>
+    </row>
+    <row r="135" ht="14.25">
+      <c r="A135" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="4"/>
+    </row>
+    <row r="136" ht="14.25">
+      <c r="A136" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="4"/>
+    </row>
+    <row r="137" ht="14.25">
+      <c r="A137" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B137" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="4"/>
+    </row>
+    <row r="138" ht="14.25">
+      <c r="A138" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -4587,218 +5180,247 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>376</v>
+      <c r="A1" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>378</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" ht="28.5">
+      <c r="A3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" ht="42.75">
+      <c r="A4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" ht="28.5">
+      <c r="A5" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" ht="42.75">
+      <c r="A6" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="3" ht="28.5">
-      <c r="A3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="C3" t="s">
-        <v>381</v>
-      </c>
-      <c r="D3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" ht="42.75">
-      <c r="A4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="C4" t="s">
-        <v>384</v>
-      </c>
-      <c r="D4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="5" ht="28.5">
-      <c r="A5" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="C5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="6" ht="42.75">
-      <c r="A6" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="17" t="s">
+        <v>435</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" ht="28.5">
+      <c r="A8" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" ht="28.5">
+      <c r="A9" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" ht="28.5">
+      <c r="A10" s="18" t="s">
         <v>391</v>
       </c>
-      <c r="D6" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="C7" t="s">
-        <v>387</v>
-      </c>
-      <c r="D7" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="8" ht="28.5">
-      <c r="A8" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="C8" t="s">
-        <v>396</v>
-      </c>
-      <c r="D8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="9" ht="28.5">
-      <c r="A9" s="7" t="s">
+      <c r="B10" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" ht="28.5">
+      <c r="A11" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="C9" t="s">
-        <v>399</v>
-      </c>
-      <c r="D9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="10" ht="28.5">
-      <c r="A10" s="7" t="s">
+      <c r="B11" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" ht="28.5">
+      <c r="A12" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="C10" t="s">
-        <v>401</v>
-      </c>
-      <c r="D10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="11" ht="28.5">
-      <c r="A11" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="C11" t="s">
-        <v>405</v>
-      </c>
-      <c r="D11" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="12" ht="28.5">
-      <c r="A12" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="C12" t="s">
-        <v>409</v>
-      </c>
-      <c r="D12" t="s">
-        <v>410</v>
+      <c r="B12" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="14" ht="42.75">
+      <c r="A14" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B15" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D13" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" ht="42.75">
-      <c r="A14" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="C14" t="s">
-        <v>414</v>
-      </c>
-      <c r="D14" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="17" ht="15">
+      <c r="A17" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="16"/>
-    <row r="17"/>
+      <c r="C17" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>468</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:D17" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A17"/>
+  </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
update species list with biovigilance dataset spit up individually
</commit_message>
<xml_diff>
--- a/data/raw-data/traits/Metatraits.xlsx
+++ b/data/raw-data/traits/Metatraits.xlsx
@@ -1432,7 +1432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -1453,22 +1453,16 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1506,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1519,21 +1513,12 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1550,6 +1535,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4850,11 +4838,11 @@
       <c r="B122" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C122" s="2" t="s">
         <v>383</v>
       </c>
       <c r="D122" s="2"/>
-      <c r="E122" s="7" t="s">
+      <c r="E122" s="6" t="s">
         <v>384</v>
       </c>
       <c r="F122" s="2"/>
@@ -4867,7 +4855,7 @@
       <c r="A123" t="s">
         <v>379</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="5" t="s">
         <v>385</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -4906,10 +4894,10 @@
       </c>
     </row>
     <row r="125" ht="14.25">
-      <c r="A125" s="9" t="s">
+      <c r="A125" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="B125" s="5" t="s">
         <v>392</v>
       </c>
       <c r="C125" s="2"/>
@@ -4922,10 +4910,10 @@
       <c r="H125" s="4"/>
     </row>
     <row r="126" ht="14.25">
-      <c r="A126" s="9" t="s">
+      <c r="A126" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B126" s="10" t="s">
+      <c r="B126" s="5" t="s">
         <v>394</v>
       </c>
       <c r="C126" s="2"/>
@@ -4938,10 +4926,10 @@
       <c r="H126" s="4"/>
     </row>
     <row r="127" ht="14.25">
-      <c r="A127" s="9" t="s">
+      <c r="A127" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B127" s="10" t="s">
+      <c r="B127" s="5" t="s">
         <v>395</v>
       </c>
       <c r="C127" s="2"/>
@@ -4960,10 +4948,10 @@
       <c r="H127" s="4"/>
     </row>
     <row r="128" ht="14.25">
-      <c r="A128" s="9" t="s">
+      <c r="A128" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B128" s="10" t="s">
+      <c r="B128" s="5" t="s">
         <v>399</v>
       </c>
       <c r="C128" s="2"/>
@@ -4982,10 +4970,10 @@
       <c r="H128" s="4"/>
     </row>
     <row r="129" ht="14.25">
-      <c r="A129" s="9" t="s">
+      <c r="A129" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B129" s="10" t="s">
+      <c r="B129" s="5" t="s">
         <v>401</v>
       </c>
       <c r="C129" s="2"/>
@@ -5000,17 +4988,17 @@
       <c r="H129" s="4"/>
     </row>
     <row r="130" ht="14.25">
-      <c r="A130" s="9" t="s">
+      <c r="A130" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B130" s="10" t="s">
+      <c r="B130" s="5" t="s">
         <v>403</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="E130" s="10" t="s">
+      <c r="E130" s="5" t="s">
         <v>404</v>
       </c>
       <c r="F130" s="2"/>
@@ -5018,10 +5006,10 @@
       <c r="H130" s="4"/>
     </row>
     <row r="131" ht="14.25">
-      <c r="A131" s="9" t="s">
+      <c r="A131" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B131" s="10" t="s">
+      <c r="B131" s="5" t="s">
         <v>405</v>
       </c>
       <c r="C131" s="2"/>
@@ -5036,10 +5024,10 @@
       <c r="H131" s="4"/>
     </row>
     <row r="132" ht="14.25">
-      <c r="A132" s="9" t="s">
+      <c r="A132" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B132" s="10" t="s">
+      <c r="B132" s="5" t="s">
         <v>407</v>
       </c>
       <c r="C132" s="2"/>
@@ -5056,32 +5044,32 @@
       <c r="H132" s="4"/>
     </row>
     <row r="133" ht="14.25">
-      <c r="A133" s="9" t="s">
+      <c r="A133" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="B133" s="5" t="s">
         <v>409</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E133" s="11" t="s">
+      <c r="E133" s="8" t="s">
         <v>411</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="G133" s="10" t="s">
+      <c r="G133" s="5" t="s">
         <v>413</v>
       </c>
       <c r="H133" s="4"/>
     </row>
     <row r="134" ht="14.25">
-      <c r="A134" s="9" t="s">
+      <c r="A134" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B134" s="10" t="s">
+      <c r="B134" s="5" t="s">
         <v>414</v>
       </c>
       <c r="C134" s="2"/>
@@ -5094,10 +5082,10 @@
       <c r="H134" s="4"/>
     </row>
     <row r="135" ht="14.25">
-      <c r="A135" s="9" t="s">
+      <c r="A135" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B135" s="10" t="s">
+      <c r="B135" s="5" t="s">
         <v>415</v>
       </c>
       <c r="C135" s="2"/>
@@ -5110,10 +5098,10 @@
       <c r="H135" s="4"/>
     </row>
     <row r="136" ht="14.25">
-      <c r="A136" s="9" t="s">
+      <c r="A136" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="B136" s="5" t="s">
         <v>416</v>
       </c>
       <c r="C136" s="2"/>
@@ -5126,10 +5114,10 @@
       <c r="H136" s="4"/>
     </row>
     <row r="137" ht="14.25">
-      <c r="A137" s="9" t="s">
+      <c r="A137" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B137" s="10" t="s">
+      <c r="B137" s="5" t="s">
         <v>417</v>
       </c>
       <c r="C137" s="2"/>
@@ -5142,10 +5130,10 @@
       <c r="H137" s="4"/>
     </row>
     <row r="138" ht="14.25">
-      <c r="A138" s="9" t="s">
+      <c r="A138" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="B138" s="5" t="s">
         <v>418</v>
       </c>
       <c r="C138" s="2"/>
@@ -5180,240 +5168,240 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="3" ht="28.5">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="4" ht="42.75">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>429</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="5" ht="28.5">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="6" ht="42.75">
-      <c r="A6" s="17" t="s">
+    <row r="6" ht="28.5">
+      <c r="A6" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>435</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="14" t="s">
+    <row r="7" ht="42.75">
+      <c r="A7" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="13" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="8" ht="28.5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="9" ht="28.5">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="10" ht="28.5">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="14" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="11" ht="28.5">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="13" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="12" ht="28.5">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="14" t="s">
+    <row r="13" ht="28.5">
+      <c r="A13" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="14" ht="42.75">
-      <c r="A14" s="14" t="s">
+    <row r="14" ht="28.5">
+      <c r="A14" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="13" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="13" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="14" t="s">
+    <row r="16" ht="42.75">
+      <c r="A16" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="13" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="17" ht="15">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="13" t="s">
         <v>468</v>
       </c>
     </row>

</xml_diff>